<commit_message>
generating all of the reports and outputs once
</commit_message>
<xml_diff>
--- a/data/outputs/tables/pathway_tables.xlsx
+++ b/data/outputs/tables/pathway_tables.xlsx
@@ -5125,34 +5125,34 @@
         <v>16</v>
       </c>
       <c r="B2" t="n">
-        <v>0.000000000000000000172139836217243</v>
+        <v>0.000000000000000000169549276198939</v>
       </c>
       <c r="C2" t="n">
-        <v>8.73757995735608</v>
+        <v>8.74173773987207</v>
       </c>
       <c r="D2" t="n">
-        <v>7.36848986707344</v>
+        <v>7.36527989544761</v>
       </c>
       <c r="E2" t="n">
         <v>39</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0000000000000000585275443138625</v>
+        <v>0.0000000000000000576467539076393</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0000000000000000229922763989891</v>
+        <v>0.0000000000000000226757785078213</v>
       </c>
       <c r="H2" t="n">
-        <v>8.10279473177</v>
+        <v>8.10664953421137</v>
       </c>
       <c r="I2" t="n">
-        <v>7.09043364567444</v>
+        <v>7.08734480505337</v>
       </c>
       <c r="J2" t="n">
         <v>36</v>
       </c>
       <c r="K2" t="n">
-        <v>0.00000000000000735178246769719</v>
+        <v>0.0000000000000072653813863872</v>
       </c>
       <c r="L2" t="s">
         <v>17</v>
@@ -5175,34 +5175,34 @@
         <v>20</v>
       </c>
       <c r="B3" t="n">
-        <v>0.00000000000000000145909072085259</v>
+        <v>0.00000000000000000144071566244539</v>
       </c>
       <c r="C3" t="n">
-        <v>10.2780349410184</v>
+        <v>10.2828131999403</v>
       </c>
       <c r="D3" t="n">
-        <v>4.92002614948791</v>
+        <v>4.9178828142017</v>
       </c>
       <c r="E3" t="n">
         <v>32</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00000000000000024804542254494</v>
+        <v>0.000000000000000244921662615716</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0000000000000000432457792217482</v>
+        <v>0.0000000000000000427375375669835</v>
       </c>
       <c r="H3" t="n">
-        <v>9.79963570127505</v>
+        <v>9.80418943533698</v>
       </c>
       <c r="I3" t="n">
-        <v>4.73436478535629</v>
+        <v>4.73230233064692</v>
       </c>
       <c r="J3" t="n">
         <v>30</v>
       </c>
       <c r="K3" t="n">
-        <v>0.00000000000000735178246769719</v>
+        <v>0.0000000000000072653813863872</v>
       </c>
       <c r="L3" t="s">
         <v>21</v>
@@ -5225,34 +5225,34 @@
         <v>23</v>
       </c>
       <c r="B4" t="n">
-        <v>0.000000000000000198391983625889</v>
+        <v>0.000000000000000196759022989518</v>
       </c>
       <c r="C4" t="n">
-        <v>17.7425821972735</v>
+        <v>17.7506014434643</v>
       </c>
       <c r="D4" t="n">
-        <v>1.80169971671388</v>
+        <v>1.80091483336964</v>
       </c>
       <c r="E4" t="n">
         <v>20</v>
       </c>
       <c r="F4" t="n">
-        <v>0.000000000000022484424810934</v>
+        <v>0.0000000000000222993559388121</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0000000000000271530483689331</v>
+        <v>0.0000000000000269531689900448</v>
       </c>
       <c r="H4" t="n">
-        <v>15.8107142857143</v>
+        <v>15.8178571428571</v>
       </c>
       <c r="I4" t="n">
-        <v>1.73371104815864</v>
+        <v>1.7329557830538</v>
       </c>
       <c r="J4" t="n">
         <v>18</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00000000000307734548181241</v>
+        <v>0.00000000000305469248553841</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
@@ -5275,34 +5275,34 @@
         <v>26</v>
       </c>
       <c r="B5" t="n">
-        <v>0.00000000000000256535587370901</v>
+        <v>0.00000000000000254444791949033</v>
       </c>
       <c r="C5" t="n">
-        <v>15.0991792065663</v>
+        <v>15.1060191518468</v>
       </c>
       <c r="D5" t="n">
-        <v>2.03268685988233</v>
+        <v>2.03180135046831</v>
       </c>
       <c r="E5" t="n">
         <v>20</v>
       </c>
       <c r="F5" t="n">
-        <v>0.000000000000218055249265266</v>
+        <v>0.000000000000216278073156678</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0000000000418747625632445</v>
+        <v>0.0000000000416071912895806</v>
       </c>
       <c r="H5" t="n">
-        <v>11.4082687338501</v>
+        <v>11.4134366925065</v>
       </c>
       <c r="I5" t="n">
-        <v>1.95598169535847</v>
+        <v>1.95512960139403</v>
       </c>
       <c r="J5" t="n">
         <v>16</v>
       </c>
       <c r="K5" t="n">
-        <v>0.00000000142374192715031</v>
+        <v>0.00000000141464450384574</v>
       </c>
       <c r="L5" t="s">
         <v>27</v>
@@ -5325,34 +5325,34 @@
         <v>29</v>
       </c>
       <c r="B6" t="n">
-        <v>0.00000000000000511741827282331</v>
+        <v>0.00000000000000508134382261838</v>
       </c>
       <c r="C6" t="n">
-        <v>20.197164258962</v>
+        <v>20.2062600321027</v>
       </c>
       <c r="D6" t="n">
-        <v>1.36282414469383</v>
+        <v>1.36223045088216</v>
       </c>
       <c r="E6" t="n">
         <v>17</v>
       </c>
       <c r="F6" t="n">
-        <v>0.000000000000347984442551985</v>
+        <v>0.00000000000034553137993805</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00000000000099861278175686</v>
+        <v>0.000000000000992445681497384</v>
       </c>
       <c r="H6" t="n">
-        <v>17.4098746081505</v>
+        <v>17.4177115987461</v>
       </c>
       <c r="I6" t="n">
-        <v>1.31139681847897</v>
+        <v>1.31082552820736</v>
       </c>
       <c r="J6" t="n">
         <v>15</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0000000000679056691594665</v>
+        <v>0.0000000000674863063418221</v>
       </c>
       <c r="L6" t="s">
         <v>30</v>
@@ -5375,34 +5375,34 @@
         <v>32</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0000000000000100057727278863</v>
+        <v>0.00000000000000990118828253016</v>
       </c>
       <c r="C7" t="n">
-        <v>8.77825497287523</v>
+        <v>8.78232368896926</v>
       </c>
       <c r="D7" t="n">
-        <v>4.5042492917847</v>
+        <v>4.50228708342409</v>
       </c>
       <c r="E7" t="n">
         <v>27</v>
       </c>
       <c r="F7" t="n">
-        <v>0.000000000000566993787913559</v>
+        <v>0.000000000000561067336010042</v>
       </c>
       <c r="G7" t="n">
-        <v>0.000000000000276589875293167</v>
+        <v>0.000000000000273932374044884</v>
       </c>
       <c r="H7" t="n">
-        <v>8.24484339190222</v>
+        <v>8.24866310160428</v>
       </c>
       <c r="I7" t="n">
-        <v>4.3342776203966</v>
+        <v>4.3323894576345</v>
       </c>
       <c r="J7" t="n">
         <v>25</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0000000000235101393999192</v>
+        <v>0.0000000000232842517938151</v>
       </c>
       <c r="L7" t="s">
         <v>33</v>
@@ -5425,34 +5425,34 @@
         <v>35</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0000000000000119793081331599</v>
+        <v>0.0000000000000118908058546073</v>
       </c>
       <c r="C8" t="n">
-        <v>16.7765151515152</v>
+        <v>16.7840909090909</v>
       </c>
       <c r="D8" t="n">
-        <v>1.66310743081281</v>
+        <v>1.66238292311043</v>
       </c>
       <c r="E8" t="n">
         <v>18</v>
       </c>
       <c r="F8" t="n">
-        <v>0.000000000000581852109324911</v>
+        <v>0.000000000000577553427223785</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0000000000228544736819038</v>
+        <v>0.000000000022715705466852</v>
       </c>
       <c r="H8" t="n">
-        <v>13.3998790078645</v>
+        <v>13.40592861464</v>
       </c>
       <c r="I8" t="n">
-        <v>1.60034865983874</v>
+        <v>1.59965149204966</v>
       </c>
       <c r="J8" t="n">
         <v>15</v>
       </c>
       <c r="K8" t="n">
-        <v>0.000000000863391227983031</v>
+        <v>0.000000000858148873192188</v>
       </c>
       <c r="L8" t="s">
         <v>36</v>
@@ -5475,34 +5475,34 @@
         <v>38</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0000000000000459768812447693</v>
+        <v>0.0000000000000455154165208878</v>
       </c>
       <c r="C9" t="n">
-        <v>8.55899390243902</v>
+        <v>8.56295731707317</v>
       </c>
       <c r="D9" t="n">
-        <v>4.38875572020048</v>
+        <v>4.38684382487475</v>
       </c>
       <c r="E9" t="n">
         <v>26</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0000000000019540174529027</v>
+        <v>0.00000000000193440520213773</v>
       </c>
       <c r="G9" t="n">
-        <v>0.00000000000126450751616437</v>
+        <v>0.0000000000012528845403749</v>
       </c>
       <c r="H9" t="n">
-        <v>8.00926784059314</v>
+        <v>8.0129749768304</v>
       </c>
       <c r="I9" t="n">
-        <v>4.22314229679669</v>
+        <v>4.22130254846439</v>
       </c>
       <c r="J9" t="n">
         <v>24</v>
       </c>
       <c r="K9" t="n">
-        <v>0.000000000071655425915981</v>
+        <v>0.0000000000709967906212443</v>
       </c>
       <c r="L9" t="s">
         <v>39</v>
@@ -5525,34 +5525,34 @@
         <v>41</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0000000000000536840592195712</v>
+        <v>0.0000000000000532526292695942</v>
       </c>
       <c r="C10" t="n">
-        <v>12.4815655133296</v>
+        <v>12.4872376630743</v>
       </c>
       <c r="D10" t="n">
-        <v>2.35606886031815</v>
+        <v>2.35504247440645</v>
       </c>
       <c r="E10" t="n">
         <v>20</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00000000000202806445940602</v>
+        <v>0.00000000000201176599462912</v>
       </c>
       <c r="G10" t="n">
-        <v>0.000000000426078849814624</v>
+        <v>0.000000000423403987313028</v>
       </c>
       <c r="H10" t="n">
-        <v>9.52082206598161</v>
+        <v>9.52514872904273</v>
       </c>
       <c r="I10" t="n">
-        <v>2.26716060143822</v>
+        <v>2.26617294707036</v>
       </c>
       <c r="J10" t="n">
         <v>16</v>
       </c>
       <c r="K10" t="n">
-        <v>0.00000000940276297793459</v>
+        <v>0.00000000929417377987699</v>
       </c>
       <c r="L10" t="s">
         <v>42</v>
@@ -5575,34 +5575,34 @@
         <v>44</v>
       </c>
       <c r="B11" t="n">
-        <v>0.000000000000111587396630443</v>
+        <v>0.000000000000110732369101754</v>
       </c>
       <c r="C11" t="n">
-        <v>13.0119602360982</v>
+        <v>13.0178626902765</v>
       </c>
       <c r="D11" t="n">
-        <v>2.14818043146655</v>
+        <v>2.14724460901764</v>
       </c>
       <c r="E11" t="n">
         <v>19</v>
       </c>
       <c r="F11" t="n">
-        <v>0.00000000000379397148543506</v>
+        <v>0.00000000000376490054945963</v>
       </c>
       <c r="G11" t="n">
-        <v>0.000000000100645368698754</v>
+        <v>0.000000000100006284072005</v>
       </c>
       <c r="H11" t="n">
-        <v>10.6553911205074</v>
+        <v>10.6602234974328</v>
       </c>
       <c r="I11" t="n">
-        <v>2.06711701895838</v>
+        <v>2.06621651056415</v>
       </c>
       <c r="J11" t="n">
         <v>16</v>
       </c>
       <c r="K11" t="n">
-        <v>0.00000000311085685068875</v>
+        <v>0.00000000309110332586196</v>
       </c>
       <c r="L11" t="s">
         <v>45</v>
@@ -5625,34 +5625,34 @@
         <v>47</v>
       </c>
       <c r="B12" t="n">
-        <v>0.000000000000126851224122848</v>
+        <v>0.000000000000125793450687541</v>
       </c>
       <c r="C12" t="n">
-        <v>10.9404634581105</v>
+        <v>10.9454545454545</v>
       </c>
       <c r="D12" t="n">
-        <v>2.77184571802136</v>
+        <v>2.77063820518406</v>
       </c>
       <c r="E12" t="n">
         <v>21</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00000000000392085601834258</v>
+        <v>0.00000000000388816120306944</v>
       </c>
       <c r="G12" t="n">
-        <v>0.00000000000670904108120844</v>
+        <v>0.00000000000665886613285624</v>
       </c>
       <c r="H12" t="n">
-        <v>9.94083263748062</v>
+        <v>9.94536562089944</v>
       </c>
       <c r="I12" t="n">
-        <v>2.66724776639791</v>
+        <v>2.66608582008277</v>
       </c>
       <c r="J12" t="n">
         <v>19</v>
       </c>
       <c r="K12" t="n">
-        <v>0.000000000285134245951359</v>
+        <v>0.00000000028300181064639</v>
       </c>
       <c r="L12" t="s">
         <v>48</v>
@@ -5675,34 +5675,34 @@
         <v>50</v>
       </c>
       <c r="B13" t="n">
-        <v>0.000000000000142327452195251</v>
+        <v>0.000000000000140909084837953</v>
       </c>
       <c r="C13" t="n">
-        <v>8.09682080924856</v>
+        <v>8.10057803468208</v>
       </c>
       <c r="D13" t="n">
-        <v>4.59664414905208</v>
+        <v>4.59464169026356</v>
       </c>
       <c r="E13" t="n">
         <v>26</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00000000000403261114553212</v>
+        <v>0.00000000000399242407040867</v>
       </c>
       <c r="G13" t="n">
-        <v>0.00000000018776523896788</v>
+        <v>0.000000000186223225780211</v>
       </c>
       <c r="H13" t="n">
-        <v>6.69632768361582</v>
+        <v>6.69943502824859</v>
       </c>
       <c r="I13" t="n">
-        <v>4.42318587927653</v>
+        <v>4.42125898497059</v>
       </c>
       <c r="J13" t="n">
         <v>22</v>
       </c>
       <c r="K13" t="n">
-        <v>0.00000000494087226601749</v>
+        <v>0.00000000489444321208393</v>
       </c>
       <c r="L13" t="s">
         <v>51</v>
@@ -5725,34 +5725,34 @@
         <v>53</v>
       </c>
       <c r="B14" t="n">
-        <v>0.00000000000362105369026057</v>
+        <v>0.0000000000035963054430394</v>
       </c>
       <c r="C14" t="n">
-        <v>12.4016853932584</v>
+        <v>12.4073033707865</v>
       </c>
       <c r="D14" t="n">
-        <v>1.96339071693179</v>
+        <v>1.96253539533871</v>
       </c>
       <c r="E14" t="n">
         <v>17</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0000000000947044811298918</v>
+        <v>0.0000000000940572192794919</v>
       </c>
       <c r="G14" t="n">
-        <v>0.000000000280992829895235</v>
+        <v>0.000000000279315966943765</v>
       </c>
       <c r="H14" t="n">
-        <v>10.8793103448276</v>
+        <v>10.884236453202</v>
       </c>
       <c r="I14" t="n">
-        <v>1.88930050119852</v>
+        <v>1.88847745589196</v>
       </c>
       <c r="J14" t="n">
         <v>15</v>
       </c>
       <c r="K14" t="n">
-        <v>0.00000000682411158316999</v>
+        <v>0.0000000067833877686343</v>
       </c>
       <c r="L14" t="s">
         <v>54</v>
@@ -5775,34 +5775,34 @@
         <v>56</v>
       </c>
       <c r="B15" t="n">
-        <v>0.000000000011642950154213</v>
+        <v>0.0000000000115639556684553</v>
       </c>
       <c r="C15" t="n">
-        <v>11.3806559368357</v>
+        <v>11.3858184026723</v>
       </c>
       <c r="D15" t="n">
-        <v>2.10198300283286</v>
+        <v>2.10106730559791</v>
       </c>
       <c r="E15" t="n">
         <v>17</v>
       </c>
       <c r="F15" t="n">
-        <v>0.00000000028275736088803</v>
+        <v>0.000000000280838923376772</v>
       </c>
       <c r="G15" t="n">
-        <v>0.00000000000609135068009252</v>
+        <v>0.00000000000604985369922802</v>
       </c>
       <c r="H15" t="n">
-        <v>11.927027027027</v>
+        <v>11.9324324324324</v>
       </c>
       <c r="I15" t="n">
-        <v>2.02266288951841</v>
+        <v>2.0217817468961</v>
       </c>
       <c r="J15" t="n">
         <v>17</v>
       </c>
       <c r="K15" t="n">
-        <v>0.000000000285134245951359</v>
+        <v>0.00000000028300181064639</v>
       </c>
       <c r="L15" t="s">
         <v>57</v>
@@ -5825,34 +5825,34 @@
         <v>59</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0000000000152814128185327</v>
+        <v>0.0000000000150856834608554</v>
       </c>
       <c r="C16" t="n">
-        <v>4.74712533842969</v>
+        <v>4.74948240165631</v>
       </c>
       <c r="D16" t="n">
-        <v>11.3645674438876</v>
+        <v>11.3596166412546</v>
       </c>
       <c r="E16" t="n">
         <v>37</v>
       </c>
       <c r="F16" t="n">
-        <v>0.000000000346378690553409</v>
+        <v>0.000000000341942158446056</v>
       </c>
       <c r="G16" t="n">
-        <v>0.00000000044248296366751</v>
+        <v>0.000000000437372883758917</v>
       </c>
       <c r="H16" t="n">
-        <v>4.39847161572052</v>
+        <v>4.40065502183406</v>
       </c>
       <c r="I16" t="n">
-        <v>10.9357158422314</v>
+        <v>10.9309518623394</v>
       </c>
       <c r="J16" t="n">
         <v>34</v>
       </c>
       <c r="K16" t="n">
-        <v>0.00000000940276297793459</v>
+        <v>0.00000000929417377987699</v>
       </c>
       <c r="L16" t="s">
         <v>60</v>
@@ -5875,34 +5875,34 @@
         <v>62</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0000000000755008044207499</v>
+        <v>0.0000000000750458683613398</v>
       </c>
       <c r="C17" t="n">
-        <v>12.1510989010989</v>
+        <v>12.1565934065934</v>
       </c>
       <c r="D17" t="n">
-        <v>1.73240357376335</v>
+        <v>1.73164887824003</v>
       </c>
       <c r="E17" t="n">
         <v>15</v>
       </c>
       <c r="F17" t="n">
-        <v>0.00000000160439209394094</v>
+        <v>0.00000000159472470267847</v>
       </c>
       <c r="G17" t="n">
-        <v>0.00000000603124005319422</v>
+        <v>0.00000000600013515900138</v>
       </c>
       <c r="H17" t="n">
-        <v>10.4249728162378</v>
+        <v>10.4296846683581</v>
       </c>
       <c r="I17" t="n">
-        <v>1.66702985399869</v>
+        <v>1.66630363755173</v>
       </c>
       <c r="J17" t="n">
         <v>13</v>
       </c>
       <c r="K17" t="n">
-        <v>0.000000107927453583475</v>
+        <v>0.000000107370839687393</v>
       </c>
       <c r="L17" t="s">
         <v>63</v>
@@ -5925,34 +5925,34 @@
         <v>65</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0000000000841451498680608</v>
+        <v>0.0000000000833240190587934</v>
       </c>
       <c r="C18" t="n">
-        <v>5.66671630677588</v>
+        <v>5.66939687267312</v>
       </c>
       <c r="D18" t="n">
-        <v>6.51383743735019</v>
+        <v>6.51099978218253</v>
       </c>
       <c r="E18" t="n">
         <v>27</v>
       </c>
       <c r="F18" t="n">
-        <v>0.00000000168290299736122</v>
+        <v>0.00000000166648038117587</v>
       </c>
       <c r="G18" t="n">
-        <v>0.000000000188915704288904</v>
+        <v>0.00000000018714047575615</v>
       </c>
       <c r="H18" t="n">
-        <v>5.65409128289474</v>
+        <v>5.65676398026316</v>
       </c>
       <c r="I18" t="n">
-        <v>6.26803225103508</v>
+        <v>6.26530167719451</v>
       </c>
       <c r="J18" t="n">
         <v>26</v>
       </c>
       <c r="K18" t="n">
-        <v>0.00000000494087226601749</v>
+        <v>0.00000000489444321208393</v>
       </c>
       <c r="L18" t="s">
         <v>66</v>
@@ -5975,34 +5975,34 @@
         <v>68</v>
       </c>
       <c r="B19" t="n">
-        <v>0.0000000000922988039156487</v>
+        <v>0.0000000000917434235893456</v>
       </c>
       <c r="C19" t="n">
-        <v>11.949198342641</v>
+        <v>11.9546027742749</v>
       </c>
       <c r="D19" t="n">
-        <v>1.75550228808019</v>
+        <v>1.7547375299499</v>
       </c>
       <c r="E19" t="n">
         <v>15</v>
       </c>
       <c r="F19" t="n">
-        <v>0.00000000174342185174003</v>
+        <v>0.00000000173293133446542</v>
       </c>
       <c r="G19" t="n">
-        <v>0.00000000714355101891745</v>
+        <v>0.00000000710676739975719</v>
       </c>
       <c r="H19" t="n">
-        <v>10.2571785268414</v>
+        <v>10.2618155876583</v>
       </c>
       <c r="I19" t="n">
-        <v>1.68925691871868</v>
+        <v>1.68852101938575</v>
       </c>
       <c r="J19" t="n">
         <v>13</v>
       </c>
       <c r="K19" t="n">
-        <v>0.000000115657492687235</v>
+        <v>0.000000115061948377021</v>
       </c>
       <c r="L19" t="s">
         <v>69</v>
@@ -6025,34 +6025,34 @@
         <v>71</v>
       </c>
       <c r="B20" t="n">
-        <v>0.000000000118436159204026</v>
+        <v>0.000000000117765328191035</v>
       </c>
       <c r="C20" t="n">
-        <v>13.2242114236999</v>
+        <v>13.230179028133</v>
       </c>
       <c r="D20" t="n">
-        <v>1.5014164305949</v>
+        <v>1.50076236114136</v>
       </c>
       <c r="E20" t="n">
         <v>14</v>
       </c>
       <c r="F20" t="n">
-        <v>0.00000000211938390154574</v>
+        <v>0.00000000210737955710273</v>
       </c>
       <c r="G20" t="n">
-        <v>0.000000125344952645952</v>
+        <v>0.000000124799735320605</v>
       </c>
       <c r="H20" t="n">
-        <v>9.92328042328042</v>
+        <v>9.92775742775743</v>
       </c>
       <c r="I20" t="n">
-        <v>1.44475920679887</v>
+        <v>1.4441298192115</v>
       </c>
       <c r="J20" t="n">
         <v>11</v>
       </c>
       <c r="K20" t="n">
-        <v>0.00000152204585355799</v>
+        <v>0.00000151542535746449</v>
       </c>
       <c r="L20" t="s">
         <v>72</v>
@@ -6075,34 +6075,34 @@
         <v>74</v>
       </c>
       <c r="B21" t="n">
-        <v>0.000000000336510328367612</v>
+        <v>0.000000000334734179884373</v>
       </c>
       <c r="C21" t="n">
-        <v>13.7859020310633</v>
+        <v>13.7921146953405</v>
       </c>
       <c r="D21" t="n">
-        <v>1.33972543037699</v>
+        <v>1.33914179917229</v>
       </c>
       <c r="E21" t="n">
         <v>13</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0000000057206755822494</v>
+        <v>0.00000000569048105803434</v>
       </c>
       <c r="G21" t="n">
-        <v>0.000000405625991080109</v>
+        <v>0.000000404018397487936</v>
       </c>
       <c r="H21" t="n">
-        <v>10.0520833333333</v>
+        <v>10.0566123188406</v>
       </c>
       <c r="I21" t="n">
-        <v>1.28916975375899</v>
+        <v>1.28860814637334</v>
       </c>
       <c r="J21" t="n">
         <v>10</v>
       </c>
       <c r="K21" t="n">
-        <v>0.00000417917687779506</v>
+        <v>0.00000416261379229994</v>
       </c>
       <c r="L21" t="s">
         <v>75</v>
@@ -6125,34 +6125,34 @@
         <v>77</v>
       </c>
       <c r="B22" t="n">
-        <v>0.000000000486107705109494</v>
+        <v>0.000000000483059350717516</v>
       </c>
       <c r="C22" t="n">
-        <v>9.4243641231593</v>
+        <v>9.42864792503347</v>
       </c>
       <c r="D22" t="n">
-        <v>2.28677271736762</v>
+        <v>2.28577651927685</v>
       </c>
       <c r="E22" t="n">
         <v>16</v>
       </c>
       <c r="F22" t="n">
-        <v>0.00000000784734044383032</v>
+        <v>0.00000000780335452904793</v>
       </c>
       <c r="G22" t="n">
-        <v>0.000000189679688830656</v>
+        <v>0.00000018873835360138</v>
       </c>
       <c r="H22" t="n">
-        <v>7.47491507708388</v>
+        <v>7.47831199372877</v>
       </c>
       <c r="I22" t="n">
-        <v>2.20047940727827</v>
+        <v>2.19952080156829</v>
       </c>
       <c r="J22" t="n">
         <v>13</v>
       </c>
       <c r="K22" t="n">
-        <v>0.00000208035787749752</v>
+        <v>0.00000207003355562803</v>
       </c>
       <c r="L22" t="s">
         <v>78</v>
@@ -6175,34 +6175,34 @@
         <v>80</v>
       </c>
       <c r="B23" t="n">
-        <v>0.000000000507769087541962</v>
+        <v>0.000000000504922940114866</v>
       </c>
       <c r="C23" t="n">
-        <v>11.609820089955</v>
+        <v>11.6150674662669</v>
       </c>
       <c r="D23" t="n">
-        <v>1.66310743081281</v>
+        <v>1.66238292311043</v>
       </c>
       <c r="E23" t="n">
         <v>14</v>
       </c>
       <c r="F23" t="n">
-        <v>0.00000000784734044383032</v>
+        <v>0.00000000780335452904793</v>
       </c>
       <c r="G23" t="n">
-        <v>0.0000000384203809207011</v>
+        <v>0.0000000382383856653135</v>
       </c>
       <c r="H23" t="n">
-        <v>9.83777777777778</v>
+        <v>9.84222222222222</v>
       </c>
       <c r="I23" t="n">
-        <v>1.60034865983874</v>
+        <v>1.59965149204966</v>
       </c>
       <c r="J23" t="n">
         <v>12</v>
       </c>
       <c r="K23" t="n">
-        <v>0.000000544288729709933</v>
+        <v>0.000000541710463591941</v>
       </c>
       <c r="L23" t="s">
         <v>81</v>
@@ -6225,34 +6225,34 @@
         <v>83</v>
       </c>
       <c r="B24" t="n">
-        <v>0.000000000608993565633306</v>
+        <v>0.000000000604234890813668</v>
       </c>
       <c r="C24" t="n">
-        <v>6.54781667268134</v>
+        <v>6.55084806928907</v>
       </c>
       <c r="D24" t="n">
-        <v>4.25016343429941</v>
+        <v>4.24831191461555</v>
       </c>
       <c r="E24" t="n">
         <v>21</v>
       </c>
       <c r="F24" t="n">
-        <v>0.00000000900251357892714</v>
+        <v>0.00000000893216795115857</v>
       </c>
       <c r="G24" t="n">
-        <v>0.0000000742808571292062</v>
+        <v>0.0000000737967274864521</v>
       </c>
       <c r="H24" t="n">
-        <v>5.57788296041308</v>
+        <v>5.58046471600688</v>
       </c>
       <c r="I24" t="n">
-        <v>4.08977990847679</v>
+        <v>4.08799825746025</v>
       </c>
       <c r="J24" t="n">
         <v>18</v>
       </c>
       <c r="K24" t="n">
-        <v>0.00000093538857125667</v>
+        <v>0.000000929292123903471</v>
       </c>
       <c r="L24" t="s">
         <v>84</v>
@@ -6275,34 +6275,34 @@
         <v>86</v>
       </c>
       <c r="B25" t="n">
-        <v>0.00000000108201431693281</v>
+        <v>0.00000000107598585153132</v>
       </c>
       <c r="C25" t="n">
-        <v>10.8509817671809</v>
+        <v>10.8558906030856</v>
       </c>
       <c r="D25" t="n">
-        <v>1.75550228808019</v>
+        <v>1.7547375299499</v>
       </c>
       <c r="E25" t="n">
         <v>14</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0000000153285361565481</v>
+        <v>0.0000000152431328966937</v>
       </c>
       <c r="G25" t="n">
-        <v>0.00000000714355101891745</v>
+        <v>0.00000000710676739975719</v>
       </c>
       <c r="H25" t="n">
-        <v>10.2571785268414</v>
+        <v>10.2618155876583</v>
       </c>
       <c r="I25" t="n">
-        <v>1.68925691871868</v>
+        <v>1.68852101938575</v>
       </c>
       <c r="J25" t="n">
         <v>13</v>
       </c>
       <c r="K25" t="n">
-        <v>0.000000115657492687235</v>
+        <v>0.000000115061948377021</v>
       </c>
       <c r="L25" t="s">
         <v>87</v>
@@ -6325,34 +6325,34 @@
         <v>89</v>
       </c>
       <c r="B26" t="n">
-        <v>0.00000000118839059275614</v>
+        <v>0.00000000117952461835656</v>
       </c>
       <c r="C26" t="n">
-        <v>6.62637698898409</v>
+        <v>6.62943696450428</v>
       </c>
       <c r="D26" t="n">
-        <v>3.97297886249728</v>
+        <v>3.97124809409715</v>
       </c>
       <c r="E26" t="n">
         <v>20</v>
       </c>
       <c r="F26" t="n">
-        <v>0.0000000161621120614834</v>
+        <v>0.0000000160415348096492</v>
       </c>
       <c r="G26" t="n">
-        <v>0.000000154417274930411</v>
+        <v>0.000000153465600152715</v>
       </c>
       <c r="H26" t="n">
-        <v>5.58967741935484</v>
+        <v>5.59225806451613</v>
       </c>
       <c r="I26" t="n">
-        <v>3.823055131837</v>
+        <v>3.82138967545197</v>
       </c>
       <c r="J26" t="n">
         <v>17</v>
       </c>
       <c r="K26" t="n">
-        <v>0.00000181040943021861</v>
+        <v>0.00000179925186385942</v>
       </c>
       <c r="L26" t="s">
         <v>90</v>
@@ -6375,34 +6375,34 @@
         <v>92</v>
       </c>
       <c r="B27" t="n">
-        <v>0.00000000173142712804615</v>
+        <v>0.00000000171961039596028</v>
       </c>
       <c r="C27" t="n">
-        <v>7.31166169895678</v>
+        <v>7.31501490312966</v>
       </c>
       <c r="D27" t="n">
-        <v>3.23382000435825</v>
+        <v>3.2324112393814</v>
       </c>
       <c r="E27" t="n">
         <v>18</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0000000226417393667574</v>
+        <v>0.0000000224872128702498</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0000000482081029432575</v>
+        <v>0.0000000479202026341981</v>
       </c>
       <c r="H27" t="n">
-        <v>6.54613653413353</v>
+        <v>6.54913728432108</v>
       </c>
       <c r="I27" t="n">
-        <v>3.11178906079756</v>
+        <v>3.11043345676323</v>
       </c>
       <c r="J27" t="n">
         <v>16</v>
       </c>
       <c r="K27" t="n">
-        <v>0.000000630413653873367</v>
+        <v>0.000000626648803677975</v>
       </c>
       <c r="L27" t="s">
         <v>93</v>
@@ -6425,34 +6425,34 @@
         <v>95</v>
       </c>
       <c r="B28" t="n">
-        <v>0.00000000365936567700704</v>
+        <v>0.00000000364164654626109</v>
       </c>
       <c r="C28" t="n">
-        <v>12.5900709219858</v>
+        <v>12.5957446808511</v>
       </c>
       <c r="D28" t="n">
-        <v>1.31662671606014</v>
+        <v>1.31605314746243</v>
       </c>
       <c r="E28" t="n">
         <v>12</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0000000460809011178664</v>
+        <v>0.0000000458577713232877</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0000034451575541271</v>
+        <v>0.00000343300001728668</v>
       </c>
       <c r="H28" t="n">
-        <v>8.94959677419355</v>
+        <v>8.95362903225806</v>
       </c>
       <c r="I28" t="n">
-        <v>1.26694268903901</v>
+        <v>1.26639076453932</v>
       </c>
       <c r="J28" t="n">
         <v>9</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0000285695992293467</v>
+        <v>0.0000284687806311578</v>
       </c>
       <c r="L28" t="s">
         <v>96</v>
@@ -6475,34 +6475,34 @@
         <v>98</v>
       </c>
       <c r="B29" t="n">
-        <v>0.00000000482328636735293</v>
+        <v>0.00000000479073155955206</v>
       </c>
       <c r="C29" t="n">
-        <v>6.79528105482304</v>
+        <v>6.79840388619015</v>
       </c>
       <c r="D29" t="n">
-        <v>3.44170843320985</v>
+        <v>3.4402091047702</v>
       </c>
       <c r="E29" t="n">
         <v>18</v>
       </c>
       <c r="F29" t="n">
-        <v>0.000000058568477317857</v>
+        <v>0.0000000581731689374178</v>
       </c>
       <c r="G29" t="n">
-        <v>0.00000397600191798579</v>
+        <v>0.00000395611304487298</v>
       </c>
       <c r="H29" t="n">
-        <v>5.12861952861953</v>
+        <v>5.13097643097643</v>
       </c>
       <c r="I29" t="n">
-        <v>3.3118326432774</v>
+        <v>3.31038989326944</v>
       </c>
       <c r="J29" t="n">
         <v>14</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0000321866821932183</v>
+        <v>0.0000320256770299241</v>
       </c>
       <c r="L29" t="s">
         <v>99</v>
@@ -6525,34 +6525,34 @@
         <v>101</v>
       </c>
       <c r="B30" t="n">
-        <v>0.00000000910501576546606</v>
+        <v>0.00000000905237237398958</v>
       </c>
       <c r="C30" t="n">
-        <v>8.13804173354735</v>
+        <v>8.14174589455488</v>
       </c>
       <c r="D30" t="n">
-        <v>2.40226628895184</v>
+        <v>2.40121977782618</v>
       </c>
       <c r="E30" t="n">
         <v>15</v>
       </c>
       <c r="F30" t="n">
-        <v>0.000000106748460698568</v>
+        <v>0.00000010613126231574</v>
       </c>
       <c r="G30" t="n">
-        <v>0.000000342150204752451</v>
+        <v>0.000000340466092483087</v>
       </c>
       <c r="H30" t="n">
-        <v>7.0561797752809</v>
+        <v>7.05939004815409</v>
       </c>
       <c r="I30" t="n">
-        <v>2.31161473087819</v>
+        <v>2.3106077107384</v>
       </c>
       <c r="J30" t="n">
         <v>13</v>
       </c>
       <c r="K30" t="n">
-        <v>0.00000363534592549479</v>
+        <v>0.0000036174522326328</v>
       </c>
       <c r="L30" t="s">
         <v>102</v>
@@ -6575,34 +6575,34 @@
         <v>104</v>
       </c>
       <c r="B31" t="n">
-        <v>0.0000000119112179431749</v>
+        <v>0.000000011842550586492</v>
       </c>
       <c r="C31" t="n">
-        <v>7.95556092259389</v>
+        <v>7.95918367346939</v>
       </c>
       <c r="D31" t="n">
-        <v>2.44846371758553</v>
+        <v>2.44739708124592</v>
       </c>
       <c r="E31" t="n">
         <v>15</v>
       </c>
       <c r="F31" t="n">
-        <v>0.000000134993803355982</v>
+        <v>0.000000134215573313576</v>
       </c>
       <c r="G31" t="n">
-        <v>0.000000429010912581067</v>
+        <v>0.000000426906233434664</v>
       </c>
       <c r="H31" t="n">
-        <v>6.90129273891507</v>
+        <v>6.90443397366195</v>
       </c>
       <c r="I31" t="n">
-        <v>2.35606886031815</v>
+        <v>2.35504247440645</v>
       </c>
       <c r="J31" t="n">
         <v>13</v>
       </c>
       <c r="K31" t="n">
-        <v>0.00000429010912581067</v>
+        <v>0.00000426906233434664</v>
       </c>
       <c r="L31" t="s">
         <v>105</v>
@@ -6625,34 +6625,34 @@
         <v>107</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0000000131087421429537</v>
+        <v>0.0000000130136806693763</v>
       </c>
       <c r="C32" t="n">
-        <v>5.65760084088819</v>
+        <v>5.66022861647615</v>
       </c>
       <c r="D32" t="n">
-        <v>4.55044672041839</v>
+        <v>4.54846438684382</v>
       </c>
       <c r="E32" t="n">
         <v>20</v>
       </c>
       <c r="F32" t="n">
-        <v>0.000000143773300922718</v>
+        <v>0.000000142730691212514</v>
       </c>
       <c r="G32" t="n">
-        <v>0.00000109658205168155</v>
+        <v>0.00000109004656048745</v>
       </c>
       <c r="H32" t="n">
-        <v>4.78555555555556</v>
+        <v>4.78777777777778</v>
       </c>
       <c r="I32" t="n">
-        <v>4.37873174983657</v>
+        <v>4.37682422130255</v>
       </c>
       <c r="J32" t="n">
         <v>17</v>
       </c>
       <c r="K32" t="n">
-        <v>0.00000981152362030857</v>
+        <v>0.00000975304817278249</v>
       </c>
       <c r="L32" t="s">
         <v>108</v>
@@ -6675,34 +6675,34 @@
         <v>110</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0000000173957217694098</v>
+        <v>0.0000000173245732098162</v>
       </c>
       <c r="C33" t="n">
-        <v>14.9596774193548</v>
+        <v>14.9663978494624</v>
       </c>
       <c r="D33" t="n">
-        <v>0.94704728699063</v>
+        <v>0.946634720104552</v>
       </c>
       <c r="E33" t="n">
         <v>10</v>
       </c>
       <c r="F33" t="n">
-        <v>0.000000184114777725202</v>
+        <v>0.000000183235730825227</v>
       </c>
       <c r="G33" t="n">
-        <v>0.000000180209597518044</v>
+        <v>0.000000179550339062576</v>
       </c>
       <c r="H33" t="n">
-        <v>13.4727822580645</v>
+        <v>13.4788306451613</v>
       </c>
       <c r="I33" t="n">
-        <v>0.911309653519285</v>
+        <v>0.910912655194947</v>
       </c>
       <c r="J33" t="n">
         <v>9</v>
       </c>
       <c r="K33" t="n">
-        <v>0.00000204237543853783</v>
+        <v>0.00000203490384270919</v>
       </c>
       <c r="L33" t="s">
         <v>111</v>
@@ -6725,34 +6725,34 @@
         <v>113</v>
       </c>
       <c r="B34" t="n">
-        <v>0.0000000178699637203873</v>
+        <v>0.0000000177846444624485</v>
       </c>
       <c r="C34" t="n">
-        <v>10.6704134885588</v>
+        <v>10.6752308309916</v>
       </c>
       <c r="D34" t="n">
-        <v>1.5014164305949</v>
+        <v>1.50076236114136</v>
       </c>
       <c r="E34" t="n">
         <v>12</v>
       </c>
       <c r="F34" t="n">
-        <v>0.000000184114777725202</v>
+        <v>0.000000183235730825227</v>
       </c>
       <c r="G34" t="n">
-        <v>0.0000105628052457649</v>
+        <v>0.0000105262132572266</v>
       </c>
       <c r="H34" t="n">
-        <v>7.65725806451613</v>
+        <v>7.66071428571429</v>
       </c>
       <c r="I34" t="n">
-        <v>1.44475920679887</v>
+        <v>1.4441298192115</v>
       </c>
       <c r="J34" t="n">
         <v>9</v>
       </c>
       <c r="K34" t="n">
-        <v>0.000078072908338262</v>
+        <v>0.0000778024458142836</v>
       </c>
       <c r="L34" t="s">
         <v>114</v>
@@ -6775,34 +6775,34 @@
         <v>116</v>
       </c>
       <c r="B35" t="n">
-        <v>0.000000020663905928593</v>
+        <v>0.0000000205391876125513</v>
       </c>
       <c r="C35" t="n">
-        <v>7.0022022022022</v>
+        <v>7.00540540540541</v>
       </c>
       <c r="D35" t="n">
-        <v>2.93353671823927</v>
+        <v>2.93225876715313</v>
       </c>
       <c r="E35" t="n">
         <v>16</v>
       </c>
       <c r="F35" t="n">
-        <v>0.00000020663905928593</v>
+        <v>0.000000205391876125513</v>
       </c>
       <c r="G35" t="n">
-        <v>0.000000567996643744338</v>
+        <v>0.000000565053583313699</v>
       </c>
       <c r="H35" t="n">
-        <v>6.1580852775543</v>
+        <v>6.1609010458568</v>
       </c>
       <c r="I35" t="n">
-        <v>2.82283721943779</v>
+        <v>2.82160749292093</v>
       </c>
       <c r="J35" t="n">
         <v>14</v>
       </c>
       <c r="K35" t="n">
-        <v>0.00000551768168208786</v>
+        <v>0.00000548909195219022</v>
       </c>
       <c r="L35" t="s">
         <v>117</v>
@@ -6825,34 +6825,34 @@
         <v>119</v>
       </c>
       <c r="B36" t="n">
-        <v>0.0000000398325672595996</v>
+        <v>0.0000000395823237630908</v>
       </c>
       <c r="C36" t="n">
-        <v>6.19931242663089</v>
+        <v>6.20216334060037</v>
       </c>
       <c r="D36" t="n">
-        <v>3.48790586184354</v>
+        <v>3.48638640818994</v>
       </c>
       <c r="E36" t="n">
         <v>17</v>
       </c>
       <c r="F36" t="n">
-        <v>0.000000386944939093253</v>
+        <v>0.000000384514002270024</v>
       </c>
       <c r="G36" t="n">
-        <v>0.0000000219270419514546</v>
+        <v>0.0000000217881845613766</v>
       </c>
       <c r="H36" t="n">
-        <v>6.49701492537313</v>
+        <v>6.5</v>
       </c>
       <c r="I36" t="n">
-        <v>3.35628677271737</v>
+        <v>3.35482465693749</v>
       </c>
       <c r="J36" t="n">
         <v>17</v>
       </c>
       <c r="K36" t="n">
-        <v>0.000000338872466522481</v>
+        <v>0.00000033672648867582</v>
       </c>
       <c r="L36" t="s">
         <v>120</v>
@@ -6875,34 +6875,34 @@
         <v>122</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0000000485817512252372</v>
+        <v>0.00000004827736194253</v>
       </c>
       <c r="C37" t="n">
-        <v>6.10533707865169</v>
+        <v>6.10814606741573</v>
       </c>
       <c r="D37" t="n">
-        <v>3.53410329047723</v>
+        <v>3.53256371160967</v>
       </c>
       <c r="E37" t="n">
         <v>17</v>
       </c>
       <c r="F37" t="n">
-        <v>0.000000458827650460573</v>
+        <v>0.000000455952862790562</v>
       </c>
       <c r="G37" t="n">
-        <v>0.0000000267887374569442</v>
+        <v>0.0000000266195243206873</v>
       </c>
       <c r="H37" t="n">
-        <v>6.39852941176471</v>
+        <v>6.40147058823529</v>
       </c>
       <c r="I37" t="n">
-        <v>3.40074090215733</v>
+        <v>3.39925942060553</v>
       </c>
       <c r="J37" t="n">
         <v>17</v>
       </c>
       <c r="K37" t="n">
-        <v>0.000000396007423276567</v>
+        <v>0.000000393506011697117</v>
       </c>
       <c r="L37" t="s">
         <v>123</v>
@@ -6925,34 +6925,34 @@
         <v>125</v>
       </c>
       <c r="B38" t="n">
-        <v>0.0000000542769476001432</v>
+        <v>0.0000000540033081936633</v>
       </c>
       <c r="C38" t="n">
-        <v>8.44454264250994</v>
+        <v>8.44837236706437</v>
       </c>
       <c r="D38" t="n">
-        <v>1.98648943124864</v>
+        <v>1.98562404704857</v>
       </c>
       <c r="E38" t="n">
         <v>13</v>
       </c>
       <c r="F38" t="n">
-        <v>0.000000498761140109424</v>
+        <v>0.000000496246615833663</v>
       </c>
       <c r="G38" t="n">
-        <v>0.00000000352544358553489</v>
+        <v>0.00000000350600526850723</v>
       </c>
       <c r="H38" t="n">
-        <v>9.75536616161616</v>
+        <v>9.75978535353535</v>
       </c>
       <c r="I38" t="n">
-        <v>1.9115275659185</v>
+        <v>1.91069483772599</v>
       </c>
       <c r="J38" t="n">
         <v>14</v>
       </c>
       <c r="K38" t="n">
-        <v>0.0000000705088717106978</v>
+        <v>0.0000000701201053701446</v>
       </c>
       <c r="L38" t="s">
         <v>126</v>
@@ -6975,34 +6975,34 @@
         <v>128</v>
       </c>
       <c r="B39" t="n">
-        <v>0.0000000593588465664584</v>
+        <v>0.0000000590231659024437</v>
       </c>
       <c r="C39" t="n">
-        <v>6.94051141166526</v>
+        <v>6.94368131868132</v>
       </c>
       <c r="D39" t="n">
-        <v>2.74874700370451</v>
+        <v>2.74754955347419</v>
       </c>
       <c r="E39" t="n">
         <v>15</v>
       </c>
       <c r="F39" t="n">
-        <v>0.000000531105469278838</v>
+        <v>0.000000528102010706076</v>
       </c>
       <c r="G39" t="n">
-        <v>0.00000000444364431207039</v>
+        <v>0.00000000441635415022018</v>
       </c>
       <c r="H39" t="n">
-        <v>7.91871754346354</v>
+        <v>7.92233009708738</v>
       </c>
       <c r="I39" t="n">
-        <v>2.64502070167793</v>
+        <v>2.64386843824875</v>
       </c>
       <c r="J39" t="n">
         <v>16</v>
       </c>
       <c r="K39" t="n">
-        <v>0.0000000839355036724407</v>
+        <v>0.0000000834200228374923</v>
       </c>
       <c r="L39" t="s">
         <v>129</v>
@@ -7025,34 +7025,34 @@
         <v>131</v>
       </c>
       <c r="B40" t="n">
-        <v>0.0000000733185239867105</v>
+        <v>0.000000072927367126233</v>
       </c>
       <c r="C40" t="n">
-        <v>7.42777777777778</v>
+        <v>7.43115942028986</v>
       </c>
       <c r="D40" t="n">
-        <v>2.40226628895184</v>
+        <v>2.40121977782618</v>
       </c>
       <c r="E40" t="n">
         <v>14</v>
       </c>
       <c r="F40" t="n">
-        <v>0.000000639187132191835</v>
+        <v>0.000000635777046741518</v>
       </c>
       <c r="G40" t="n">
-        <v>0.0000000444454190436669</v>
+        <v>0.0000000442068284545712</v>
       </c>
       <c r="H40" t="n">
-        <v>7.77247474747475</v>
+        <v>7.7760101010101</v>
       </c>
       <c r="I40" t="n">
-        <v>2.31161473087819</v>
+        <v>2.3106077107384</v>
       </c>
       <c r="J40" t="n">
         <v>14</v>
       </c>
       <c r="K40" t="n">
-        <v>0.00000060445769899387</v>
+        <v>0.000000601212866982168</v>
       </c>
       <c r="L40" t="s">
         <v>132</v>
@@ -7075,34 +7075,34 @@
         <v>134</v>
       </c>
       <c r="B41" t="n">
-        <v>0.0000000934522992004191</v>
+        <v>0.0000000928993139560013</v>
       </c>
       <c r="C41" t="n">
-        <v>6.19804444444444</v>
+        <v>6.20088888888889</v>
       </c>
       <c r="D41" t="n">
-        <v>3.25691871867509</v>
+        <v>3.25549989109127</v>
       </c>
       <c r="E41" t="n">
         <v>16</v>
       </c>
       <c r="F41" t="n">
-        <v>0.000000794344543203562</v>
+        <v>0.000000789644168626011</v>
       </c>
       <c r="G41" t="n">
-        <v>0.0000111855445299578</v>
+        <v>0.000011133859012802</v>
       </c>
       <c r="H41" t="n">
-        <v>4.97428019662921</v>
+        <v>4.9765625</v>
       </c>
       <c r="I41" t="n">
-        <v>3.13401612551754</v>
+        <v>3.13265083859726</v>
       </c>
       <c r="J41" t="n">
         <v>13</v>
       </c>
       <c r="K41" t="n">
-        <v>0.0000809167051103333</v>
+        <v>0.0000805428098798444</v>
       </c>
       <c r="L41" t="s">
         <v>135</v>
@@ -7125,34 +7125,34 @@
         <v>137</v>
       </c>
       <c r="B42" t="n">
-        <v>0.000000124095712853003</v>
+        <v>0.000000123476387689143</v>
       </c>
       <c r="C42" t="n">
-        <v>7.79256839526337</v>
+        <v>7.79610725466177</v>
       </c>
       <c r="D42" t="n">
-        <v>2.12508171714971</v>
+        <v>2.12415595730778</v>
       </c>
       <c r="E42" t="n">
         <v>13</v>
       </c>
       <c r="F42" t="n">
-        <v>0.00000102908639926881</v>
+        <v>0.00000102395053205631</v>
       </c>
       <c r="G42" t="n">
-        <v>0.0000299173056251073</v>
+        <v>0.0000298069834898949</v>
       </c>
       <c r="H42" t="n">
-        <v>5.83907741251326</v>
+        <v>5.84172852598091</v>
       </c>
       <c r="I42" t="n">
-        <v>2.0448899542384</v>
+        <v>2.04399912873012</v>
       </c>
       <c r="J42" t="n">
         <v>10</v>
       </c>
       <c r="K42" t="n">
-        <v>0.000175377308836836</v>
+        <v>0.000174730592871797</v>
       </c>
       <c r="L42" t="s">
         <v>138</v>
@@ -7175,34 +7175,34 @@
         <v>140</v>
       </c>
       <c r="B43" t="n">
-        <v>0.000000158526068807977</v>
+        <v>0.000000157838257518565</v>
       </c>
       <c r="C43" t="n">
-        <v>9.67825223435948</v>
+        <v>9.68262164846077</v>
       </c>
       <c r="D43" t="n">
-        <v>1.47831771627806</v>
+        <v>1.4776737094315</v>
       </c>
       <c r="E43" t="n">
         <v>11</v>
       </c>
       <c r="F43" t="n">
-        <v>0.00000128330627130267</v>
+        <v>0.00000127773827515029</v>
       </c>
       <c r="G43" t="n">
-        <v>0.00000105402123408457</v>
+        <v>0.00000104989517943222</v>
       </c>
       <c r="H43" t="n">
-        <v>8.92310789049919</v>
+        <v>8.92713365539453</v>
       </c>
       <c r="I43" t="n">
-        <v>1.42253214207888</v>
+        <v>1.42191243737748</v>
       </c>
       <c r="J43" t="n">
         <v>10</v>
       </c>
       <c r="K43" t="n">
-        <v>0.00000968560052942578</v>
+        <v>0.00000964768543262041</v>
       </c>
       <c r="L43" t="s">
         <v>141</v>
@@ -7225,34 +7225,34 @@
         <v>143</v>
       </c>
       <c r="B44" t="n">
-        <v>0.000000200318521850842</v>
+        <v>0.000000199387566609689</v>
       </c>
       <c r="C44" t="n">
-        <v>8.28848560700876</v>
+        <v>8.29224030037547</v>
       </c>
       <c r="D44" t="n">
-        <v>1.84789714534757</v>
+        <v>1.84709213678937</v>
       </c>
       <c r="E44" t="n">
         <v>12</v>
       </c>
       <c r="F44" t="n">
-        <v>0.00000158391389370433</v>
+        <v>0.00000157655285226266</v>
       </c>
       <c r="G44" t="n">
-        <v>0.000349347351767009</v>
+        <v>0.000348333003503325</v>
       </c>
       <c r="H44" t="n">
-        <v>5.21867612293144</v>
+        <v>5.2210401891253</v>
       </c>
       <c r="I44" t="n">
-        <v>1.77816517759861</v>
+        <v>1.77739054672185</v>
       </c>
       <c r="J44" t="n">
         <v>8</v>
       </c>
       <c r="K44" t="n">
-        <v>0.00154257272208809</v>
+        <v>0.00153809378170299</v>
       </c>
       <c r="L44" t="s">
         <v>144</v>
@@ -7275,34 +7275,34 @@
         <v>146</v>
       </c>
       <c r="B45" t="n">
-        <v>0.00000020775249616002</v>
+        <v>0.000000206722710263922</v>
       </c>
       <c r="C45" t="n">
-        <v>7.41028630651639</v>
+        <v>7.4136546184739</v>
       </c>
       <c r="D45" t="n">
-        <v>2.21747657441708</v>
+        <v>2.21651056414724</v>
       </c>
       <c r="E45" t="n">
         <v>13</v>
       </c>
       <c r="F45" t="n">
-        <v>0.00000160536019760016</v>
+        <v>0.00000159740276113031</v>
       </c>
       <c r="G45" t="n">
-        <v>0.0000434681527027645</v>
+        <v>0.000043309269652832</v>
       </c>
       <c r="H45" t="n">
-        <v>5.56243680485339</v>
+        <v>5.5649646107179</v>
       </c>
       <c r="I45" t="n">
-        <v>2.13379821311833</v>
+        <v>2.13286865606622</v>
       </c>
       <c r="J45" t="n">
         <v>10</v>
       </c>
       <c r="K45" t="n">
-        <v>0.000242281506867868</v>
+        <v>0.000241395929212506</v>
       </c>
       <c r="L45" t="s">
         <v>147</v>
@@ -7325,34 +7325,34 @@
         <v>149</v>
       </c>
       <c r="B46" t="n">
-        <v>0.000000212845899719113</v>
+        <v>0.000000211726592655461</v>
       </c>
       <c r="C46" t="n">
-        <v>6.73869126043039</v>
+        <v>6.74176548089592</v>
       </c>
       <c r="D46" t="n">
-        <v>2.61015471780344</v>
+        <v>2.60901764321499</v>
       </c>
       <c r="E46" t="n">
         <v>14</v>
       </c>
       <c r="F46" t="n">
-        <v>0.00000160816902009996</v>
+        <v>0.00000159971203339681</v>
       </c>
       <c r="G46" t="n">
-        <v>0.000000909982245688357</v>
+        <v>0.000000905569781653896</v>
       </c>
       <c r="H46" t="n">
-        <v>6.40797752808989</v>
+        <v>6.41089887640449</v>
       </c>
       <c r="I46" t="n">
-        <v>2.51165831335803</v>
+        <v>2.51056414724461</v>
       </c>
       <c r="J46" t="n">
         <v>13</v>
       </c>
       <c r="K46" t="n">
-        <v>0.00000859427676483448</v>
+        <v>0.00000855260349339791</v>
       </c>
       <c r="L46" t="s">
         <v>150</v>
@@ -7375,34 +7375,34 @@
         <v>152</v>
       </c>
       <c r="B47" t="n">
-        <v>0.000000295275934854854</v>
+        <v>0.000000293558715514789</v>
       </c>
       <c r="C47" t="n">
-        <v>5.63957826439578</v>
+        <v>5.64217356042174</v>
       </c>
       <c r="D47" t="n">
-        <v>3.53410329047723</v>
+        <v>3.53256371160967</v>
       </c>
       <c r="E47" t="n">
         <v>16</v>
       </c>
       <c r="F47" t="n">
-        <v>0.00000218247430110109</v>
+        <v>0.0000021697818103267</v>
       </c>
       <c r="G47" t="n">
-        <v>0.00000544448025014613</v>
+        <v>0.00000541742349041364</v>
       </c>
       <c r="H47" t="n">
-        <v>4.97645519947678</v>
+        <v>4.97874427730543</v>
       </c>
       <c r="I47" t="n">
-        <v>3.40074090215733</v>
+        <v>3.39925942060553</v>
       </c>
       <c r="J47" t="n">
         <v>14</v>
       </c>
       <c r="K47" t="n">
-        <v>0.0000430493787220857</v>
+        <v>0.0000428354415521078</v>
       </c>
       <c r="L47" t="s">
         <v>153</v>
@@ -7425,34 +7425,34 @@
         <v>155</v>
       </c>
       <c r="B48" t="n">
-        <v>0.000000397331664915527</v>
+        <v>0.000000395501963994365</v>
       </c>
       <c r="C48" t="n">
-        <v>7.71203730690761</v>
+        <v>7.71553482949577</v>
       </c>
       <c r="D48" t="n">
-        <v>1.96339071693179</v>
+        <v>1.96253539533871</v>
       </c>
       <c r="E48" t="n">
         <v>12</v>
       </c>
       <c r="F48" t="n">
-        <v>0.00000287431417172934</v>
+        <v>0.00000286107803740605</v>
       </c>
       <c r="G48" t="n">
-        <v>0.0000941086732378617</v>
+        <v>0.0000937978443128376</v>
       </c>
       <c r="H48" t="n">
-        <v>5.61672325976231</v>
+        <v>5.61926994906621</v>
       </c>
       <c r="I48" t="n">
-        <v>1.88930050119852</v>
+        <v>1.88847745589196</v>
       </c>
       <c r="J48" t="n">
         <v>9</v>
       </c>
       <c r="K48" t="n">
-        <v>0.000484802256073833</v>
+        <v>0.000483201016157042</v>
       </c>
       <c r="L48" t="s">
         <v>156</v>
@@ -7475,34 +7475,34 @@
         <v>158</v>
       </c>
       <c r="B49" t="n">
-        <v>0.000000817982925915065</v>
+        <v>0.000000812862596909846</v>
       </c>
       <c r="C49" t="n">
-        <v>4.64718614718615</v>
+        <v>4.64935064935065</v>
       </c>
       <c r="D49" t="n">
-        <v>4.78143386358684</v>
+        <v>4.7793509039425</v>
       </c>
       <c r="E49" t="n">
         <v>18</v>
       </c>
       <c r="F49" t="n">
-        <v>0.00000579404572523171</v>
+        <v>0.00000575777672811141</v>
       </c>
       <c r="G49" t="n">
-        <v>0.00000996572932562222</v>
+        <v>0.00000991165086316362</v>
       </c>
       <c r="H49" t="n">
-        <v>4.18458541336905</v>
+        <v>4.18653354438086</v>
       </c>
       <c r="I49" t="n">
-        <v>4.60100239703639</v>
+        <v>4.59899803964278</v>
       </c>
       <c r="J49" t="n">
         <v>16</v>
       </c>
       <c r="K49" t="n">
-        <v>0.0000752966215713679</v>
+        <v>0.0000748880287439029</v>
       </c>
       <c r="L49" t="s">
         <v>159</v>
@@ -7525,34 +7525,34 @@
         <v>161</v>
       </c>
       <c r="B50" t="n">
-        <v>0.00000134548450041391</v>
+        <v>0.00000133861459026391</v>
       </c>
       <c r="C50" t="n">
-        <v>5.67855815681903</v>
+        <v>5.68115942028986</v>
       </c>
       <c r="D50" t="n">
-        <v>3.02593157550665</v>
+        <v>3.02461337399259</v>
       </c>
       <c r="E50" t="n">
         <v>14</v>
       </c>
       <c r="F50" t="n">
-        <v>0.00000933601490083121</v>
+        <v>0.00000928834613652511</v>
       </c>
       <c r="G50" t="n">
-        <v>0.000131272506194921</v>
+        <v>0.000130771913908427</v>
       </c>
       <c r="H50" t="n">
-        <v>4.39899267399267</v>
+        <v>4.40100732600733</v>
       </c>
       <c r="I50" t="n">
-        <v>2.91174547831772</v>
+        <v>2.91047702025702</v>
       </c>
       <c r="J50" t="n">
         <v>11</v>
       </c>
       <c r="K50" t="n">
-        <v>0.000614464241490044</v>
+        <v>0.000611810805107249</v>
       </c>
       <c r="L50" t="s">
         <v>162</v>
@@ -7575,34 +7575,34 @@
         <v>164</v>
       </c>
       <c r="B51" t="n">
-        <v>0.0000016188698606645</v>
+        <v>0.0000016106316101961</v>
       </c>
       <c r="C51" t="n">
-        <v>5.58056265984655</v>
+        <v>5.58312020460358</v>
       </c>
       <c r="D51" t="n">
-        <v>3.07212900414034</v>
+        <v>3.07079067741233</v>
       </c>
       <c r="E51" t="n">
         <v>14</v>
       </c>
       <c r="F51" t="n">
-        <v>0.0000110083150525186</v>
+        <v>0.0000109522949493335</v>
       </c>
       <c r="G51" t="n">
-        <v>0.0000311378833627073</v>
+        <v>0.0000310058371626483</v>
       </c>
       <c r="H51" t="n">
-        <v>4.81101928374656</v>
+        <v>4.81322314049587</v>
       </c>
       <c r="I51" t="n">
-        <v>2.95619960775768</v>
+        <v>2.95491178392507</v>
       </c>
       <c r="J51" t="n">
         <v>12</v>
       </c>
       <c r="K51" t="n">
-        <v>0.000179438649886788</v>
+        <v>0.000178677705683058</v>
       </c>
       <c r="L51" t="s">
         <v>165</v>
@@ -7625,34 +7625,34 @@
         <v>167</v>
       </c>
       <c r="B52" t="n">
-        <v>0.00000234613971690693</v>
+        <v>0.00000233494873224821</v>
       </c>
       <c r="C52" t="n">
-        <v>5.82836661546339</v>
+        <v>5.8310291858679</v>
       </c>
       <c r="D52" t="n">
-        <v>2.72564828938767</v>
+        <v>2.72446090176432</v>
       </c>
       <c r="E52" t="n">
         <v>13</v>
       </c>
       <c r="F52" t="n">
-        <v>0.0000156409314460462</v>
+        <v>0.0000155663248816548</v>
       </c>
       <c r="G52" t="n">
-        <v>0.00000913643192575708</v>
+        <v>0.00000909657020384145</v>
       </c>
       <c r="H52" t="n">
-        <v>5.51069182389937</v>
+        <v>5.51320754716981</v>
       </c>
       <c r="I52" t="n">
-        <v>2.62279363695794</v>
+        <v>2.62165105641472</v>
       </c>
       <c r="J52" t="n">
         <v>12</v>
       </c>
       <c r="K52" t="n">
-        <v>0.0000705997012444865</v>
+        <v>0.0000702916788478658</v>
       </c>
       <c r="L52" t="s">
         <v>168</v>
@@ -7675,34 +7675,34 @@
         <v>170</v>
       </c>
       <c r="B53" t="n">
-        <v>0.00000268177913845407</v>
+        <v>0.00000267142331857005</v>
       </c>
       <c r="C53" t="n">
-        <v>7.94719827586207</v>
+        <v>7.95079022988506</v>
       </c>
       <c r="D53" t="n">
-        <v>1.57071257354543</v>
+        <v>1.57002831627096</v>
       </c>
       <c r="E53" t="n">
         <v>10</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0000175347097514305</v>
+        <v>0.0000174669986214196</v>
       </c>
       <c r="G53" t="n">
-        <v>0.0000154075892226047</v>
+        <v>0.000015354587103233</v>
       </c>
       <c r="H53" t="n">
-        <v>7.26298523783488</v>
+        <v>7.26626571897212</v>
       </c>
       <c r="I53" t="n">
-        <v>1.51144040095881</v>
+        <v>1.51078196471357</v>
       </c>
       <c r="J53" t="n">
         <v>9</v>
       </c>
       <c r="K53" t="n">
-        <v>0.0000988411384091624</v>
+        <v>0.000098501124813193</v>
       </c>
       <c r="L53" t="s">
         <v>171</v>
@@ -7725,34 +7725,34 @@
         <v>173</v>
       </c>
       <c r="B54" t="n">
-        <v>0.00000307646808118722</v>
+        <v>0.00000306461417799783</v>
       </c>
       <c r="C54" t="n">
-        <v>7.81073446327684</v>
+        <v>7.81426553672316</v>
       </c>
       <c r="D54" t="n">
-        <v>1.59381128786228</v>
+        <v>1.59311696798083</v>
       </c>
       <c r="E54" t="n">
         <v>10</v>
       </c>
       <c r="F54" t="n">
-        <v>0.0000197358329736539</v>
+        <v>0.0000196597890664012</v>
       </c>
       <c r="G54" t="n">
-        <v>0.000123274956472844</v>
+        <v>0.000122906186110087</v>
       </c>
       <c r="H54" t="n">
-        <v>6.17509591907918</v>
+        <v>6.17788629229159</v>
       </c>
       <c r="I54" t="n">
-        <v>1.5336674656788</v>
+        <v>1.53299934654759</v>
       </c>
       <c r="J54" t="n">
         <v>8</v>
       </c>
       <c r="K54" t="n">
-        <v>0.000590330777475591</v>
+        <v>0.000588564834893375</v>
       </c>
       <c r="L54" t="s">
         <v>174</v>
@@ -7775,34 +7775,34 @@
         <v>176</v>
       </c>
       <c r="B55" t="n">
-        <v>0.00000315608886764188</v>
+        <v>0.00000314597430561771</v>
       </c>
       <c r="C55" t="n">
-        <v>11.0080395794682</v>
+        <v>11.012987012987</v>
       </c>
       <c r="D55" t="n">
-        <v>0.94704728699063</v>
+        <v>0.946634720104552</v>
       </c>
       <c r="E55" t="n">
         <v>8</v>
       </c>
       <c r="F55" t="n">
-        <v>0.0000198716706481155</v>
+        <v>0.0000198079863687041</v>
       </c>
       <c r="G55" t="n">
-        <v>0.00000235534317968973</v>
+        <v>0.00000234776787159694</v>
       </c>
       <c r="H55" t="n">
-        <v>11.4867827208253</v>
+        <v>11.49194068343</v>
       </c>
       <c r="I55" t="n">
-        <v>0.911309653519285</v>
+        <v>0.910912655194947</v>
       </c>
       <c r="J55" t="n">
         <v>8</v>
       </c>
       <c r="K55" t="n">
-        <v>0.0000200204170273627</v>
+        <v>0.000019956026908574</v>
       </c>
       <c r="L55" t="s">
         <v>177</v>
@@ -7825,34 +7825,34 @@
         <v>179</v>
       </c>
       <c r="B56" t="n">
-        <v>0.00000362089477365245</v>
+        <v>0.00000360480470884448</v>
       </c>
       <c r="C56" t="n">
-        <v>6.09296947271045</v>
+        <v>6.09574468085106</v>
       </c>
       <c r="D56" t="n">
-        <v>2.40226628895184</v>
+        <v>2.40121977782618</v>
       </c>
       <c r="E56" t="n">
         <v>12</v>
       </c>
       <c r="F56" t="n">
-        <v>0.0000223837131462152</v>
+        <v>0.0000222842472910386</v>
       </c>
       <c r="G56" t="n">
-        <v>0.000015201673772143</v>
+        <v>0.0000151403674123121</v>
       </c>
       <c r="H56" t="n">
-        <v>5.71121351766513</v>
+        <v>5.71381306865178</v>
       </c>
       <c r="I56" t="n">
-        <v>2.31161473087819</v>
+        <v>2.3106077107384</v>
       </c>
       <c r="J56" t="n">
         <v>11</v>
       </c>
       <c r="K56" t="n">
-        <v>0.0000988411384091624</v>
+        <v>0.000098501124813193</v>
       </c>
       <c r="L56" t="s">
         <v>180</v>
@@ -7875,34 +7875,34 @@
         <v>182</v>
       </c>
       <c r="B57" t="n">
-        <v>0.00000400459145746674</v>
+        <v>0.00000398347586006257</v>
       </c>
       <c r="C57" t="n">
-        <v>4.79460137178258</v>
+        <v>4.7968139243307</v>
       </c>
       <c r="D57" t="n">
-        <v>3.78818914796252</v>
+        <v>3.78653888041821</v>
       </c>
       <c r="E57" t="n">
         <v>15</v>
       </c>
       <c r="F57" t="n">
-        <v>0.0000243135909917623</v>
+        <v>0.0000241853891503799</v>
       </c>
       <c r="G57" t="n">
-        <v>0.000922643081957122</v>
+        <v>0.00091937181096663</v>
       </c>
       <c r="H57" t="n">
-        <v>3.42411836529484</v>
+        <v>3.42569848452201</v>
       </c>
       <c r="I57" t="n">
-        <v>3.64523861407714</v>
+        <v>3.64365062077979</v>
       </c>
       <c r="J57" t="n">
         <v>11</v>
       </c>
       <c r="K57" t="n">
-        <v>0.00364765869610955</v>
+        <v>0.00363472576428668</v>
       </c>
       <c r="L57" t="s">
         <v>183</v>
@@ -7925,34 +7925,34 @@
         <v>185</v>
       </c>
       <c r="B58" t="n">
-        <v>0.00000412260791555224</v>
+        <v>0.00000410315365714174</v>
       </c>
       <c r="C58" t="n">
-        <v>5.50576382834447</v>
+        <v>5.50828247602441</v>
       </c>
       <c r="D58" t="n">
-        <v>2.86424057528873</v>
+        <v>2.86299281202352</v>
       </c>
       <c r="E58" t="n">
         <v>13</v>
       </c>
       <c r="F58" t="n">
-        <v>0.0000245909945839958</v>
+        <v>0.0000244749516390911</v>
       </c>
       <c r="G58" t="n">
-        <v>0.0000152647795808263</v>
+        <v>0.0000151989265041763</v>
       </c>
       <c r="H58" t="n">
-        <v>5.20833333333333</v>
+        <v>5.21071428571429</v>
       </c>
       <c r="I58" t="n">
-        <v>2.75615602527784</v>
+        <v>2.75495534741886</v>
       </c>
       <c r="J58" t="n">
         <v>12</v>
       </c>
       <c r="K58" t="n">
-        <v>0.0000988411384091624</v>
+        <v>0.000098501124813193</v>
       </c>
       <c r="L58" t="s">
         <v>186</v>
@@ -7975,34 +7975,34 @@
         <v>188</v>
       </c>
       <c r="B59" t="n">
-        <v>0.00000457838919784078</v>
+        <v>0.00000455555802054672</v>
       </c>
       <c r="C59" t="n">
-        <v>5.05542648523067</v>
+        <v>5.05774975107866</v>
       </c>
       <c r="D59" t="n">
-        <v>3.34931357594247</v>
+        <v>3.34785449793073</v>
       </c>
       <c r="E59" t="n">
         <v>14</v>
       </c>
       <c r="F59" t="n">
-        <v>0.0000263839377502689</v>
+        <v>0.0000262523682539981</v>
       </c>
       <c r="G59" t="n">
-        <v>0.0000734602682198517</v>
+        <v>0.0000731559339331705</v>
       </c>
       <c r="H59" t="n">
-        <v>4.36491228070175</v>
+        <v>4.36691729323308</v>
       </c>
       <c r="I59" t="n">
-        <v>3.22292438439747</v>
+        <v>3.22152036593335</v>
       </c>
       <c r="J59" t="n">
         <v>12</v>
       </c>
       <c r="K59" t="n">
-        <v>0.000390257674917962</v>
+        <v>0.000388640899019968</v>
       </c>
       <c r="L59" t="s">
         <v>189</v>
@@ -8025,34 +8025,34 @@
         <v>191</v>
       </c>
       <c r="B60" t="n">
-        <v>0.00000457838919784078</v>
+        <v>0.00000455555802054672</v>
       </c>
       <c r="C60" t="n">
-        <v>5.05542648523067</v>
+        <v>5.05774975107866</v>
       </c>
       <c r="D60" t="n">
-        <v>3.34931357594247</v>
+        <v>3.34785449793073</v>
       </c>
       <c r="E60" t="n">
         <v>14</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0000263839377502689</v>
+        <v>0.0000262523682539981</v>
       </c>
       <c r="G60" t="n">
-        <v>0.0000151912802669865</v>
+        <v>0.0000151215813819179</v>
       </c>
       <c r="H60" t="n">
-        <v>4.81911814776983</v>
+        <v>4.82133129043241</v>
       </c>
       <c r="I60" t="n">
-        <v>3.22292438439747</v>
+        <v>3.22152036593335</v>
       </c>
       <c r="J60" t="n">
         <v>13</v>
       </c>
       <c r="K60" t="n">
-        <v>0.0000988411384091624</v>
+        <v>0.000098501124813193</v>
       </c>
       <c r="L60" t="s">
         <v>192</v>
@@ -8075,34 +8075,34 @@
         <v>194</v>
       </c>
       <c r="B61" t="n">
-        <v>0.0000048092162097261</v>
+        <v>0.00000478936925043099</v>
       </c>
       <c r="C61" t="n">
-        <v>6.5391363022942</v>
+        <v>6.54210526315789</v>
       </c>
       <c r="D61" t="n">
-        <v>2.05578557419917</v>
+        <v>2.05489000217817</v>
       </c>
       <c r="E61" t="n">
         <v>11</v>
       </c>
       <c r="F61" t="n">
-        <v>0.0000272522251884479</v>
+        <v>0.0000271397590857756</v>
       </c>
       <c r="G61" t="n">
-        <v>0.0000222998281301011</v>
+        <v>0.000022217053814661</v>
       </c>
       <c r="H61" t="n">
-        <v>6.06494221243809</v>
+        <v>6.06769400110072</v>
       </c>
       <c r="I61" t="n">
-        <v>1.97820876007845</v>
+        <v>1.97734698322805</v>
       </c>
       <c r="J61" t="n">
         <v>10</v>
       </c>
       <c r="K61" t="n">
-        <v>0.000135391813647042</v>
+        <v>0.000134889255303299</v>
       </c>
       <c r="L61" t="s">
         <v>195</v>
@@ -8125,34 +8125,34 @@
         <v>197</v>
       </c>
       <c r="B62" t="n">
-        <v>0.00000490070503703035</v>
+        <v>0.00000487905282943455</v>
       </c>
       <c r="C62" t="n">
-        <v>5.89652855543113</v>
+        <v>5.89921612541993</v>
       </c>
       <c r="D62" t="n">
-        <v>2.47156243190238</v>
+        <v>2.47048573295578</v>
       </c>
       <c r="E62" t="n">
         <v>12</v>
       </c>
       <c r="F62" t="n">
-        <v>0.0000273154051244315</v>
+        <v>0.0000271947206886516</v>
       </c>
       <c r="G62" t="n">
-        <v>0.00239761989040447</v>
+        <v>0.00239117234778036</v>
       </c>
       <c r="H62" t="n">
-        <v>3.77218998495594</v>
+        <v>3.7739093058242</v>
       </c>
       <c r="I62" t="n">
-        <v>2.37829592503813</v>
+        <v>2.37725985624047</v>
       </c>
       <c r="J62" t="n">
         <v>8</v>
       </c>
       <c r="K62" t="n">
-        <v>0.00858095539723705</v>
+        <v>0.00855787998152969</v>
       </c>
       <c r="L62" t="s">
         <v>198</v>
@@ -8175,34 +8175,34 @@
         <v>200</v>
       </c>
       <c r="B63" t="n">
-        <v>0.00000599648191023086</v>
+        <v>0.00000597183697973977</v>
       </c>
       <c r="C63" t="n">
-        <v>6.37276315789474</v>
+        <v>6.37565789473684</v>
       </c>
       <c r="D63" t="n">
-        <v>2.10198300283286</v>
+        <v>2.10106730559791</v>
       </c>
       <c r="E63" t="n">
         <v>11</v>
       </c>
       <c r="F63" t="n">
-        <v>0.0000328839330561047</v>
+        <v>0.0000327487834372826</v>
       </c>
       <c r="G63" t="n">
-        <v>0.0000271624614291924</v>
+        <v>0.0000270620778595224</v>
       </c>
       <c r="H63" t="n">
-        <v>5.91250670960816</v>
+        <v>5.91519055287171</v>
       </c>
       <c r="I63" t="n">
-        <v>2.02266288951841</v>
+        <v>2.0217817468961</v>
       </c>
       <c r="J63" t="n">
         <v>10</v>
       </c>
       <c r="K63" t="n">
-        <v>0.000162021699753077</v>
+        <v>0.000161422920565572</v>
       </c>
       <c r="L63" t="s">
         <v>201</v>
@@ -8225,34 +8225,34 @@
         <v>203</v>
       </c>
       <c r="B64" t="n">
-        <v>0.00000915947702343174</v>
+        <v>0.00000912214322504531</v>
       </c>
       <c r="C64" t="n">
-        <v>6.06378446115288</v>
+        <v>6.06654135338346</v>
       </c>
       <c r="D64" t="n">
-        <v>2.19437786010024</v>
+        <v>2.19342191243738</v>
       </c>
       <c r="E64" t="n">
         <v>11</v>
       </c>
       <c r="F64" t="n">
-        <v>0.0000494320982216951</v>
+        <v>0.0000492306142304032</v>
       </c>
       <c r="G64" t="n">
-        <v>0.0000396660441370763</v>
+        <v>0.0000395207370464062</v>
       </c>
       <c r="H64" t="n">
-        <v>5.62915601023018</v>
+        <v>5.63171355498721</v>
       </c>
       <c r="I64" t="n">
-        <v>2.11157114839834</v>
+        <v>2.11065127423219</v>
       </c>
       <c r="J64" t="n">
         <v>10</v>
       </c>
       <c r="K64" t="n">
-        <v>0.000224774250110099</v>
+        <v>0.000223950843262969</v>
       </c>
       <c r="L64" t="s">
         <v>204</v>
@@ -8275,34 +8275,34 @@
         <v>206</v>
       </c>
       <c r="B65" t="n">
-        <v>0.0000110365887169821</v>
+        <v>0.0000109797134468303</v>
       </c>
       <c r="C65" t="n">
-        <v>4.36863749747185</v>
+        <v>4.37066001483179</v>
       </c>
       <c r="D65" t="n">
-        <v>4.11157114839834</v>
+        <v>4.10978000435635</v>
       </c>
       <c r="E65" t="n">
         <v>15</v>
       </c>
       <c r="F65" t="n">
-        <v>0.0000586318775589673</v>
+        <v>0.0000583297276862857</v>
       </c>
       <c r="G65" t="n">
-        <v>0.000131929087143451</v>
+        <v>0.000131359378743615</v>
       </c>
       <c r="H65" t="n">
-        <v>3.8260810350698</v>
+        <v>3.82785154919986</v>
       </c>
       <c r="I65" t="n">
-        <v>3.9564175201569</v>
+        <v>3.95469396645611</v>
       </c>
       <c r="J65" t="n">
         <v>13</v>
       </c>
       <c r="K65" t="n">
-        <v>0.000614464241490044</v>
+        <v>0.000611810805107249</v>
       </c>
       <c r="L65" t="s">
         <v>207</v>
@@ -8325,34 +8325,34 @@
         <v>209</v>
       </c>
       <c r="B66" t="n">
-        <v>0.0000186428061086931</v>
+        <v>0.0000185789025748341</v>
       </c>
       <c r="C66" t="n">
-        <v>7.07874155705652</v>
+        <v>7.08194098826875</v>
       </c>
       <c r="D66" t="n">
-        <v>1.54761385922859</v>
+        <v>1.5469396645611</v>
       </c>
       <c r="E66" t="n">
         <v>9</v>
       </c>
       <c r="F66" t="n">
-        <v>0.0000975162165685485</v>
+        <v>0.0000971819519299016</v>
       </c>
       <c r="G66" t="n">
-        <v>0.000635065063412254</v>
+        <v>0.000633433496917633</v>
       </c>
       <c r="H66" t="n">
-        <v>5.43666666666667</v>
+        <v>5.43912280701754</v>
       </c>
       <c r="I66" t="n">
-        <v>1.48921333623883</v>
+        <v>1.48856458287955</v>
       </c>
       <c r="J66" t="n">
         <v>7</v>
       </c>
       <c r="K66" t="n">
-        <v>0.0026657052044465</v>
+        <v>0.00265885665372834</v>
       </c>
       <c r="L66" t="s">
         <v>210</v>
@@ -8375,34 +8375,34 @@
         <v>212</v>
       </c>
       <c r="B67" t="n">
-        <v>0.0000201298002951522</v>
+        <v>0.0000200736654694363</v>
       </c>
       <c r="C67" t="n">
-        <v>10.1544477028348</v>
+        <v>10.159009449332</v>
       </c>
       <c r="D67" t="n">
-        <v>0.877751144040096</v>
+        <v>0.877368764974951</v>
       </c>
       <c r="E67" t="n">
         <v>7</v>
       </c>
       <c r="F67" t="n">
-        <v>0.000103698971217451</v>
+        <v>0.000103409791812247</v>
       </c>
       <c r="G67" t="n">
-        <v>0.00000127384784089307</v>
+        <v>0.00000126972009375424</v>
       </c>
       <c r="H67" t="n">
-        <v>12.6439716312057</v>
+        <v>12.6496453900709</v>
       </c>
       <c r="I67" t="n">
-        <v>0.844628459359338</v>
+        <v>0.844260509692877</v>
       </c>
       <c r="J67" t="n">
         <v>8</v>
       </c>
       <c r="K67" t="n">
-        <v>0.0000111053401513755</v>
+        <v>0.0000110693546634985</v>
       </c>
       <c r="L67" t="s">
         <v>213</v>
@@ -8425,34 +8425,34 @@
         <v>215</v>
       </c>
       <c r="B68" t="n">
-        <v>0.0000208007343125381</v>
+        <v>0.0000207234018167725</v>
       </c>
       <c r="C68" t="n">
-        <v>6.12222222222222</v>
+        <v>6.125</v>
       </c>
       <c r="D68" t="n">
-        <v>1.96339071693179</v>
+        <v>1.96253539533871</v>
       </c>
       <c r="E68" t="n">
         <v>10</v>
       </c>
       <c r="F68" t="n">
-        <v>0.000105555965168104</v>
+        <v>0.000105163531607502</v>
       </c>
       <c r="G68" t="n">
-        <v>0.0000941086732378617</v>
+        <v>0.0000937978443128376</v>
       </c>
       <c r="H68" t="n">
-        <v>5.61672325976231</v>
+        <v>5.61926994906621</v>
       </c>
       <c r="I68" t="n">
-        <v>1.88930050119852</v>
+        <v>1.88847745589196</v>
       </c>
       <c r="J68" t="n">
         <v>9</v>
       </c>
       <c r="K68" t="n">
-        <v>0.000484802256073833</v>
+        <v>0.000483201016157042</v>
       </c>
       <c r="L68" t="s">
         <v>216</v>
@@ -8475,34 +8475,34 @@
         <v>218</v>
       </c>
       <c r="B69" t="n">
-        <v>0.0000258270597625746</v>
+        <v>0.0000256968356895534</v>
       </c>
       <c r="C69" t="n">
-        <v>4.03377872127872</v>
+        <v>4.03565184815185</v>
       </c>
       <c r="D69" t="n">
-        <v>4.41185443451732</v>
+        <v>4.40993247658462</v>
       </c>
       <c r="E69" t="n">
         <v>15</v>
       </c>
       <c r="F69" t="n">
-        <v>0.000129135298812873</v>
+        <v>0.000128484178447767</v>
       </c>
       <c r="G69" t="n">
-        <v>0.0000160999605566693</v>
+        <v>0.0000160177343719987</v>
       </c>
       <c r="H69" t="n">
-        <v>4.22315830721003</v>
+        <v>4.22511755485893</v>
       </c>
       <c r="I69" t="n">
-        <v>4.24536936151667</v>
+        <v>4.24351993029841</v>
       </c>
       <c r="J69" t="n">
         <v>15</v>
       </c>
       <c r="K69" t="n">
-        <v>0.000101370122023473</v>
+        <v>0.000100852401601473</v>
       </c>
       <c r="L69" t="s">
         <v>219</v>
@@ -8525,34 +8525,34 @@
         <v>221</v>
       </c>
       <c r="B70" t="n">
-        <v>0.0000310388259428361</v>
+        <v>0.0000308989656872968</v>
       </c>
       <c r="C70" t="n">
-        <v>4.46797912713472</v>
+        <v>4.47003478810879</v>
       </c>
       <c r="D70" t="n">
-        <v>3.44170843320985</v>
+        <v>3.4402091047702</v>
       </c>
       <c r="E70" t="n">
         <v>13</v>
       </c>
       <c r="F70" t="n">
-        <v>0.000152944939428468</v>
+        <v>0.000152255772951897</v>
       </c>
       <c r="G70" t="n">
-        <v>0.0000957977674951618</v>
+        <v>0.0000954040176249579</v>
       </c>
       <c r="H70" t="n">
-        <v>4.23357664233577</v>
+        <v>4.23552311435523</v>
       </c>
       <c r="I70" t="n">
-        <v>3.3118326432774</v>
+        <v>3.31038989326944</v>
       </c>
       <c r="J70" t="n">
         <v>12</v>
       </c>
       <c r="K70" t="n">
-        <v>0.000486137924602314</v>
+        <v>0.000484139790932622</v>
       </c>
       <c r="L70" t="s">
         <v>222</v>
@@ -8575,34 +8575,34 @@
         <v>224</v>
       </c>
       <c r="B71" t="n">
-        <v>0.0000410376336138993</v>
+        <v>0.0000408039527838123</v>
       </c>
       <c r="C71" t="n">
-        <v>3.39144385026738</v>
+        <v>3.39304812834225</v>
       </c>
       <c r="D71" t="n">
-        <v>6.30594900849858</v>
+        <v>6.30320191679373</v>
       </c>
       <c r="E71" t="n">
         <v>18</v>
       </c>
       <c r="F71" t="n">
-        <v>0.000199325648981796</v>
+        <v>0.000198190627807088</v>
       </c>
       <c r="G71" t="n">
-        <v>0.000895641405689937</v>
+        <v>0.000891671728464015</v>
       </c>
       <c r="H71" t="n">
-        <v>2.82611601176156</v>
+        <v>2.82745255279337</v>
       </c>
       <c r="I71" t="n">
-        <v>6.06798866855524</v>
+        <v>6.0653452406883</v>
       </c>
       <c r="J71" t="n">
         <v>15</v>
       </c>
       <c r="K71" t="n">
-        <v>0.00358256562275975</v>
+        <v>0.00356668691385606</v>
       </c>
       <c r="L71" t="s">
         <v>225</v>
@@ -8625,34 +8625,34 @@
         <v>227</v>
       </c>
       <c r="B72" t="n">
-        <v>0.0000494955365839533</v>
+        <v>0.0000492882181043108</v>
       </c>
       <c r="C72" t="n">
-        <v>4.56330659225671</v>
+        <v>4.56539937216603</v>
       </c>
       <c r="D72" t="n">
-        <v>3.09522771845718</v>
+        <v>3.0938793291222</v>
       </c>
       <c r="E72" t="n">
         <v>12</v>
       </c>
       <c r="F72" t="n">
-        <v>0.000237020879416114</v>
+        <v>0.000236028086696699</v>
       </c>
       <c r="G72" t="n">
-        <v>0.00270757891758673</v>
+        <v>0.00269969939396433</v>
       </c>
       <c r="H72" t="n">
-        <v>3.37703225806452</v>
+        <v>3.37858064516129</v>
       </c>
       <c r="I72" t="n">
-        <v>2.97842667247766</v>
+        <v>2.97712916575909</v>
       </c>
       <c r="J72" t="n">
         <v>9</v>
       </c>
       <c r="K72" t="n">
-        <v>0.00958934199978635</v>
+        <v>0.00956143535362368</v>
       </c>
       <c r="L72" t="s">
         <v>228</v>
@@ -8675,34 +8675,34 @@
         <v>230</v>
       </c>
       <c r="B73" t="n">
-        <v>0.0000587436561583032</v>
+        <v>0.0000585647434097872</v>
       </c>
       <c r="C73" t="n">
-        <v>6.95604395604396</v>
+        <v>6.95918367346939</v>
       </c>
       <c r="D73" t="n">
-        <v>1.38592285901068</v>
+        <v>1.38531910259203</v>
       </c>
       <c r="E73" t="n">
         <v>8</v>
       </c>
       <c r="F73" t="n">
-        <v>0.000277400598525321</v>
+        <v>0.000276555732768439</v>
       </c>
       <c r="G73" t="n">
-        <v>0.0000444936311743892</v>
+        <v>0.0000443573228017592</v>
       </c>
       <c r="H73" t="n">
-        <v>7.25859247135843</v>
+        <v>7.26186579378069</v>
       </c>
       <c r="I73" t="n">
-        <v>1.33362388319895</v>
+        <v>1.33304291004139</v>
       </c>
       <c r="J73" t="n">
         <v>8</v>
       </c>
       <c r="K73" t="n">
-        <v>0.000243997332246651</v>
+        <v>0.000243249834719325</v>
       </c>
       <c r="L73" t="s">
         <v>231</v>
@@ -8725,34 +8725,34 @@
         <v>233</v>
       </c>
       <c r="B74" t="n">
-        <v>0.0000643618337339964</v>
+        <v>0.0000641471710153705</v>
       </c>
       <c r="C74" t="n">
-        <v>5.9354549529359</v>
+        <v>5.93814432989691</v>
       </c>
       <c r="D74" t="n">
-        <v>1.80169971671388</v>
+        <v>1.80091483336964</v>
       </c>
       <c r="E74" t="n">
         <v>9</v>
       </c>
       <c r="F74" t="n">
-        <v>0.000299767444788476</v>
+        <v>0.000298767645825013</v>
       </c>
       <c r="G74" t="n">
-        <v>0.0073367866427032</v>
+        <v>0.00732174587375677</v>
       </c>
       <c r="H74" t="n">
-        <v>3.83246527777778</v>
+        <v>3.83420138888889</v>
       </c>
       <c r="I74" t="n">
-        <v>1.73371104815864</v>
+        <v>1.7329557830538</v>
       </c>
       <c r="J74" t="n">
         <v>6</v>
       </c>
       <c r="K74" t="n">
-        <v>0.0226773405319917</v>
+        <v>0.0226308508825209</v>
       </c>
       <c r="L74" t="s">
         <v>234</v>
@@ -8775,34 +8775,34 @@
         <v>236</v>
       </c>
       <c r="B75" t="n">
-        <v>0.0000663049546602828</v>
+        <v>0.0000659483782202354</v>
       </c>
       <c r="C75" t="n">
-        <v>3.37691947565543</v>
+        <v>3.37851123595506</v>
       </c>
       <c r="D75" t="n">
-        <v>5.93636957942907</v>
+        <v>5.93378348943585</v>
       </c>
       <c r="E75" t="n">
         <v>17</v>
       </c>
       <c r="F75" t="n">
-        <v>0.000304644386276975</v>
+        <v>0.000303006062092973</v>
       </c>
       <c r="G75" t="n">
-        <v>0.00416632137341909</v>
+        <v>0.00415102185294118</v>
       </c>
       <c r="H75" t="n">
-        <v>2.54001657763861</v>
+        <v>2.54121385153804</v>
       </c>
       <c r="I75" t="n">
-        <v>5.71235563303552</v>
+        <v>5.70986713134393</v>
       </c>
       <c r="J75" t="n">
         <v>13</v>
       </c>
       <c r="K75" t="n">
-        <v>0.0137973487380436</v>
+        <v>0.0137613333539969</v>
       </c>
       <c r="L75" t="s">
         <v>237</v>
@@ -8825,34 +8825,34 @@
         <v>239</v>
       </c>
       <c r="B76" t="n">
-        <v>0.0000790800352633419</v>
+        <v>0.0000787953864862724</v>
       </c>
       <c r="C76" t="n">
-        <v>5.14279026217228</v>
+        <v>5.14513108614232</v>
       </c>
       <c r="D76" t="n">
-        <v>2.28677271736762</v>
+        <v>2.28577651927685</v>
       </c>
       <c r="E76" t="n">
         <v>10</v>
       </c>
       <c r="F76" t="n">
-        <v>0.000353779105125477</v>
+        <v>0.000352505676385956</v>
       </c>
       <c r="G76" t="n">
-        <v>0.000305746487280897</v>
+        <v>0.000304771088846764</v>
       </c>
       <c r="H76" t="n">
-        <v>4.72795698924731</v>
+        <v>4.73010752688172</v>
       </c>
       <c r="I76" t="n">
-        <v>2.20047940727827</v>
+        <v>2.19952080156829</v>
       </c>
       <c r="J76" t="n">
         <v>9</v>
       </c>
       <c r="K76" t="n">
-        <v>0.00139308171743185</v>
+        <v>0.0013882716052338</v>
       </c>
       <c r="L76" t="s">
         <v>240</v>
@@ -8875,34 +8875,34 @@
         <v>242</v>
       </c>
       <c r="B77" t="n">
-        <v>0.0000786724222468845</v>
+        <v>0.0000783076484287944</v>
       </c>
       <c r="C77" t="n">
-        <v>3.81407987866532</v>
+        <v>3.81584934277048</v>
       </c>
       <c r="D77" t="n">
-        <v>4.2963608629331</v>
+        <v>4.29448921803529</v>
       </c>
       <c r="E77" t="n">
         <v>14</v>
       </c>
       <c r="F77" t="n">
-        <v>0.000353779105125477</v>
+        <v>0.000352505676385956</v>
       </c>
       <c r="G77" t="n">
-        <v>0.0000116716764695675</v>
+        <v>0.0000116115884898774</v>
       </c>
       <c r="H77" t="n">
-        <v>4.3516838072192</v>
+        <v>4.35370034281105</v>
       </c>
       <c r="I77" t="n">
-        <v>4.13423403791676</v>
+        <v>4.13243302112829</v>
       </c>
       <c r="J77" t="n">
         <v>15</v>
       </c>
       <c r="K77" t="n">
-        <v>0.0000826743749927699</v>
+        <v>0.0000822487518032979</v>
       </c>
       <c r="L77" t="s">
         <v>243</v>
@@ -8925,34 +8925,34 @@
         <v>245</v>
       </c>
       <c r="B78" t="n">
-        <v>0.0000817595713644522</v>
+        <v>0.000081421978412194</v>
       </c>
       <c r="C78" t="n">
-        <v>4.30875804057397</v>
+        <v>4.31073725878278</v>
       </c>
       <c r="D78" t="n">
-        <v>3.25691871867509</v>
+        <v>3.25549989109127</v>
       </c>
       <c r="E78" t="n">
         <v>12</v>
       </c>
       <c r="F78" t="n">
-        <v>0.000361016289141737</v>
+        <v>0.000359525618962935</v>
       </c>
       <c r="G78" t="n">
-        <v>0.00103677622308987</v>
+        <v>0.00103336368372674</v>
       </c>
       <c r="H78" t="n">
-        <v>3.61433786923332</v>
+        <v>3.61599734483903</v>
       </c>
       <c r="I78" t="n">
-        <v>3.13401612551754</v>
+        <v>3.13265083859726</v>
       </c>
       <c r="J78" t="n">
         <v>10</v>
       </c>
       <c r="K78" t="n">
-        <v>0.00400572631648357</v>
+        <v>0.00399254150530785</v>
       </c>
       <c r="L78" t="s">
         <v>246</v>
@@ -8975,34 +8975,34 @@
         <v>248</v>
       </c>
       <c r="B79" t="n">
-        <v>0.0000884078809209124</v>
+        <v>0.0000879994802610957</v>
       </c>
       <c r="C79" t="n">
-        <v>3.76849075462269</v>
+        <v>3.77023988005997</v>
       </c>
       <c r="D79" t="n">
-        <v>4.34255829156679</v>
+        <v>4.34066652145502</v>
       </c>
       <c r="E79" t="n">
         <v>14</v>
       </c>
       <c r="F79" t="n">
-        <v>0.000385367686065516</v>
+        <v>0.000383587478061187</v>
       </c>
       <c r="G79" t="n">
-        <v>0.0000132925293390775</v>
+        <v>0.0000132243146339923</v>
       </c>
       <c r="H79" t="n">
-        <v>4.29938210085709</v>
+        <v>4.30137532389874</v>
       </c>
       <c r="I79" t="n">
-        <v>4.17868816735672</v>
+        <v>4.17686778479634</v>
       </c>
       <c r="J79" t="n">
         <v>15</v>
       </c>
       <c r="K79" t="n">
-        <v>0.0000922338770466604</v>
+        <v>0.0000917605505215794</v>
       </c>
       <c r="L79" t="s">
         <v>249</v>
@@ -9025,34 +9025,34 @@
         <v>251</v>
       </c>
       <c r="B80" t="n">
-        <v>0.0000907100675960936</v>
+        <v>0.000090360333545158</v>
       </c>
       <c r="C80" t="n">
-        <v>4.60315789473684</v>
+        <v>4.60526315789474</v>
       </c>
       <c r="D80" t="n">
-        <v>2.7949444323382</v>
+        <v>2.79372685689392</v>
       </c>
       <c r="E80" t="n">
         <v>11</v>
       </c>
       <c r="F80" t="n">
-        <v>0.000390397759274327</v>
+        <v>0.000388892574751313</v>
       </c>
       <c r="G80" t="n">
-        <v>0.00030729743766879</v>
+        <v>0.000306236383507456</v>
       </c>
       <c r="H80" t="n">
-        <v>4.28515471993733</v>
+        <v>4.28711320015668</v>
       </c>
       <c r="I80" t="n">
-        <v>2.68947483111789</v>
+        <v>2.68830320191679</v>
       </c>
       <c r="J80" t="n">
         <v>10</v>
       </c>
       <c r="K80" t="n">
-        <v>0.00139308171743185</v>
+        <v>0.0013882716052338</v>
       </c>
       <c r="L80" t="s">
         <v>252</v>
@@ -9075,34 +9075,34 @@
         <v>254</v>
       </c>
       <c r="B81" t="n">
-        <v>0.0000977947234767287</v>
+        <v>0.0000974185032528197</v>
       </c>
       <c r="C81" t="n">
-        <v>4.5606448553817</v>
+        <v>4.56273115220484</v>
       </c>
       <c r="D81" t="n">
-        <v>2.81804314665504</v>
+        <v>2.81681550860379</v>
       </c>
       <c r="E81" t="n">
         <v>11</v>
       </c>
       <c r="F81" t="n">
-        <v>0.000415627574776097</v>
+        <v>0.000414028638824484</v>
       </c>
       <c r="G81" t="n">
-        <v>0.0000685742988378884</v>
+        <v>0.000068307782706862</v>
       </c>
       <c r="H81" t="n">
-        <v>4.76546876546877</v>
+        <v>4.76764676764677</v>
       </c>
       <c r="I81" t="n">
-        <v>2.71170189583787</v>
+        <v>2.71052058375082</v>
       </c>
       <c r="J81" t="n">
         <v>11</v>
       </c>
       <c r="K81" t="n">
-        <v>0.000370083517537811</v>
+        <v>0.000368645176513223</v>
       </c>
       <c r="L81" t="s">
         <v>255</v>
@@ -9125,34 +9125,34 @@
         <v>257</v>
       </c>
       <c r="B82" t="n">
-        <v>0.000123057641315189</v>
+        <v>0.000122525188779004</v>
       </c>
       <c r="C82" t="n">
-        <v>3.85165399630162</v>
+        <v>3.85343469625368</v>
       </c>
       <c r="D82" t="n">
-        <v>3.92678143386359</v>
+        <v>3.92507079067741</v>
       </c>
       <c r="E82" t="n">
         <v>13</v>
       </c>
       <c r="F82" t="n">
-        <v>0.000516538247495854</v>
+        <v>0.000514303261541498</v>
       </c>
       <c r="G82" t="n">
-        <v>0.00417314474585262</v>
+        <v>0.00416038042672753</v>
       </c>
       <c r="H82" t="n">
-        <v>2.93953804347826</v>
+        <v>2.94089673913043</v>
       </c>
       <c r="I82" t="n">
-        <v>3.77860100239704</v>
+        <v>3.77695491178393</v>
       </c>
       <c r="J82" t="n">
         <v>10</v>
       </c>
       <c r="K82" t="n">
-        <v>0.0137973487380436</v>
+        <v>0.0137613333539969</v>
       </c>
       <c r="L82" t="s">
         <v>258</v>
@@ -9175,34 +9175,34 @@
         <v>260</v>
       </c>
       <c r="B83" t="n">
-        <v>0.00014427023773842</v>
+        <v>0.000143883465290194</v>
       </c>
       <c r="C83" t="n">
-        <v>7.13337924701561</v>
+        <v>7.13659320477502</v>
       </c>
       <c r="D83" t="n">
-        <v>1.17803443015908</v>
+        <v>1.17752123720322</v>
       </c>
       <c r="E83" t="n">
         <v>7</v>
       </c>
       <c r="F83" t="n">
-        <v>0.000598193668671498</v>
+        <v>0.00059658997803251</v>
       </c>
       <c r="G83" t="n">
-        <v>0.000113093662624884</v>
+        <v>0.000112788791072856</v>
       </c>
       <c r="H83" t="n">
-        <v>7.44043062200957</v>
+        <v>7.44377990430622</v>
       </c>
       <c r="I83" t="n">
-        <v>1.13358030071911</v>
+        <v>1.13308647353518</v>
       </c>
       <c r="J83" t="n">
         <v>7</v>
       </c>
       <c r="K83" t="n">
-        <v>0.000549312075606581</v>
+        <v>0.000547831270925301</v>
       </c>
       <c r="L83" t="s">
         <v>261</v>
@@ -9225,34 +9225,34 @@
         <v>263</v>
       </c>
       <c r="B84" t="n">
-        <v>0.000152886941705337</v>
+        <v>0.000152346946154795</v>
       </c>
       <c r="C84" t="n">
-        <v>4.71005154639175</v>
+        <v>4.71219931271478</v>
       </c>
       <c r="D84" t="n">
-        <v>2.47156243190238</v>
+        <v>2.47048573295578</v>
       </c>
       <c r="E84" t="n">
         <v>10</v>
       </c>
       <c r="F84" t="n">
-        <v>0.000626283857588126</v>
+        <v>0.000624071827622054</v>
       </c>
       <c r="G84" t="n">
-        <v>0.000110512961914637</v>
+        <v>0.00011011886334906</v>
       </c>
       <c r="H84" t="n">
-        <v>4.91931869116988</v>
+        <v>4.92155983863738</v>
       </c>
       <c r="I84" t="n">
-        <v>2.37829592503813</v>
+        <v>2.37725985624047</v>
       </c>
       <c r="J84" t="n">
         <v>10</v>
       </c>
       <c r="K84" t="n">
-        <v>0.000544556623927196</v>
+        <v>0.000542614688966385</v>
       </c>
       <c r="L84" t="s">
         <v>264</v>
@@ -9275,34 +9275,34 @@
         <v>266</v>
       </c>
       <c r="B85" t="n">
-        <v>0.000171183913267447</v>
+        <v>0.000170780407312122</v>
       </c>
       <c r="C85" t="n">
-        <v>8.61677419354839</v>
+        <v>8.62064516129032</v>
       </c>
       <c r="D85" t="n">
-        <v>0.854652429723251</v>
+        <v>0.854280113265084</v>
       </c>
       <c r="E85" t="n">
         <v>6</v>
       </c>
       <c r="F85" t="n">
-        <v>0.000692887267987287</v>
+        <v>0.000691254029596683</v>
       </c>
       <c r="G85" t="n">
-        <v>0.00121793756605409</v>
+        <v>0.00121558682041364</v>
       </c>
       <c r="H85" t="n">
-        <v>7.17622422680412</v>
+        <v>7.17944587628866</v>
       </c>
       <c r="I85" t="n">
-        <v>0.822401394639355</v>
+        <v>0.822043127858854</v>
       </c>
       <c r="J85" t="n">
         <v>5</v>
       </c>
       <c r="K85" t="n">
-        <v>0.00455053596108123</v>
+        <v>0.00454175295539163</v>
       </c>
       <c r="L85" t="s">
         <v>267</v>
@@ -9325,34 +9325,34 @@
         <v>269</v>
       </c>
       <c r="B86" t="n">
-        <v>0.000185863192010487</v>
+        <v>0.000185162341350978</v>
       </c>
       <c r="C86" t="n">
-        <v>4.20991228070175</v>
+        <v>4.21184210526316</v>
       </c>
       <c r="D86" t="n">
-        <v>3.02593157550665</v>
+        <v>3.02461337399259</v>
       </c>
       <c r="E86" t="n">
         <v>11</v>
       </c>
       <c r="F86" t="n">
-        <v>0.000734807968413554</v>
+        <v>0.000732037163480612</v>
       </c>
       <c r="G86" t="n">
-        <v>0.00231849866221673</v>
+        <v>0.00231169603038775</v>
       </c>
       <c r="H86" t="n">
-        <v>3.46245372818614</v>
+        <v>3.46404019037546</v>
       </c>
       <c r="I86" t="n">
-        <v>2.91174547831772</v>
+        <v>2.91047702025702</v>
       </c>
       <c r="J86" t="n">
         <v>9</v>
       </c>
       <c r="K86" t="n">
-        <v>0.00847623166831924</v>
+        <v>0.00845136183152509</v>
       </c>
       <c r="L86" t="s">
         <v>270</v>
@@ -9375,34 +9375,34 @@
         <v>272</v>
       </c>
       <c r="B87" t="n">
-        <v>0.000184932262322124</v>
+        <v>0.000184439536069635</v>
       </c>
       <c r="C87" t="n">
-        <v>6.8201581027668</v>
+        <v>6.82323232323232</v>
       </c>
       <c r="D87" t="n">
-        <v>1.22423185879277</v>
+        <v>1.22369854062296</v>
       </c>
       <c r="E87" t="n">
         <v>7</v>
       </c>
       <c r="F87" t="n">
-        <v>0.000734807968413554</v>
+        <v>0.000732037163480612</v>
       </c>
       <c r="G87" t="n">
-        <v>0.0293185108205104</v>
+        <v>0.0292779859212424</v>
       </c>
       <c r="H87" t="n">
-        <v>3.69679300291545</v>
+        <v>3.69845897542691</v>
       </c>
       <c r="I87" t="n">
-        <v>1.17803443015908</v>
+        <v>1.17752123720322</v>
       </c>
       <c r="J87" t="n">
         <v>4</v>
       </c>
       <c r="K87" t="n">
-        <v>0.0791134418966153</v>
+        <v>0.0790040889938287</v>
       </c>
       <c r="L87" t="s">
         <v>273</v>
@@ -9425,34 +9425,34 @@
         <v>275</v>
       </c>
       <c r="B88" t="n">
-        <v>0.000192602151451644</v>
+        <v>0.000191926754666625</v>
       </c>
       <c r="C88" t="n">
-        <v>4.565625</v>
+        <v>4.56770833333333</v>
       </c>
       <c r="D88" t="n">
-        <v>2.54085857485291</v>
+        <v>2.53975168808538</v>
       </c>
       <c r="E88" t="n">
         <v>10</v>
       </c>
       <c r="F88" t="n">
-        <v>0.000752698063144354</v>
+        <v>0.000750058581455777</v>
       </c>
       <c r="G88" t="n">
-        <v>0.00285315337214017</v>
+        <v>0.00284554841453308</v>
       </c>
       <c r="H88" t="n">
-        <v>3.65874009178139</v>
+        <v>3.66040884438882</v>
       </c>
       <c r="I88" t="n">
-        <v>2.44497711919808</v>
+        <v>2.44391200174254</v>
       </c>
       <c r="J88" t="n">
         <v>8</v>
       </c>
       <c r="K88" t="n">
-        <v>0.0100007437786357</v>
+        <v>0.00997408722619842</v>
       </c>
       <c r="L88" t="s">
         <v>276</v>
@@ -9475,34 +9475,34 @@
         <v>278</v>
       </c>
       <c r="B89" t="n">
-        <v>0.000212044507077582</v>
+        <v>0.000211094007745874</v>
       </c>
       <c r="C89" t="n">
-        <v>3.4383295194508</v>
+        <v>3.43993135011442</v>
       </c>
       <c r="D89" t="n">
-        <v>4.7121377206363</v>
+        <v>4.7100849488129</v>
       </c>
       <c r="E89" t="n">
         <v>14</v>
       </c>
       <c r="F89" t="n">
-        <v>0.000819262868254295</v>
+        <v>0.000815590484472693</v>
       </c>
       <c r="G89" t="n">
-        <v>0.0144712101625673</v>
+        <v>0.0144308598818181</v>
       </c>
       <c r="H89" t="n">
-        <v>2.40531151949798</v>
+        <v>2.40643209323173</v>
       </c>
       <c r="I89" t="n">
-        <v>4.53432120287644</v>
+        <v>4.53234589414071</v>
       </c>
       <c r="J89" t="n">
         <v>10</v>
       </c>
       <c r="K89" t="n">
-        <v>0.041001762127274</v>
+        <v>0.0408874363318179</v>
       </c>
       <c r="L89" t="s">
         <v>279</v>
@@ -9525,34 +9525,34 @@
         <v>281</v>
       </c>
       <c r="B90" t="n">
-        <v>0.000267316078831326</v>
+        <v>0.000266779418831785</v>
       </c>
       <c r="C90" t="n">
-        <v>10.5186232909005</v>
+        <v>10.5233380480905</v>
       </c>
       <c r="D90" t="n">
-        <v>0.60056657223796</v>
+        <v>0.600304944456545</v>
       </c>
       <c r="E90" t="n">
         <v>5</v>
       </c>
       <c r="F90" t="n">
-        <v>0.00102120749216462</v>
+        <v>0.00101915733036862</v>
       </c>
       <c r="G90" t="n">
-        <v>0.0000167017572566349</v>
+        <v>0.0000166607723580089</v>
       </c>
       <c r="H90" t="n">
-        <v>13.959375</v>
+        <v>13.965625</v>
       </c>
       <c r="I90" t="n">
-        <v>0.577903682719547</v>
+        <v>0.5776519276846</v>
       </c>
       <c r="J90" t="n">
         <v>6</v>
       </c>
       <c r="K90" t="n">
-        <v>0.00010324722667738</v>
+        <v>0.000102993865485873</v>
       </c>
       <c r="L90" t="s">
         <v>282</v>
@@ -9575,34 +9575,34 @@
         <v>284</v>
       </c>
       <c r="B91" t="n">
-        <v>0.00074140982221374</v>
+        <v>0.000739312203748922</v>
       </c>
       <c r="C91" t="n">
-        <v>4.6101517530089</v>
+        <v>4.61224489795918</v>
       </c>
       <c r="D91" t="n">
-        <v>1.98648943124864</v>
+        <v>1.98562404704857</v>
       </c>
       <c r="E91" t="n">
         <v>8</v>
       </c>
       <c r="F91" t="n">
-        <v>0.00257223815870073</v>
+        <v>0.00256496070688401</v>
       </c>
       <c r="G91" t="n">
-        <v>0.000103190003323861</v>
+        <v>0.000102850011209906</v>
       </c>
       <c r="H91" t="n">
-        <v>5.5425219941349</v>
+        <v>5.54503560955174</v>
       </c>
       <c r="I91" t="n">
-        <v>1.9115275659185</v>
+        <v>1.91069483772599</v>
       </c>
       <c r="J91" t="n">
         <v>9</v>
       </c>
       <c r="K91" t="n">
-        <v>0.000515950016619306</v>
+        <v>0.000514250056049532</v>
       </c>
       <c r="L91" t="s">
         <v>285</v>

</xml_diff>